<commit_message>
renamed files, added README images, minor cleanup edits
</commit_message>
<xml_diff>
--- a/DCF valuations.xlsx
+++ b/DCF valuations.xlsx
@@ -7,18 +7,19 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="FIVN" sheetId="1" r:id="rId1"/>
-    <sheet name="ASAN" sheetId="2" r:id="rId2"/>
-    <sheet name="LPRO" sheetId="3" r:id="rId3"/>
+    <sheet name="ASAN" sheetId="1" r:id="rId1"/>
+    <sheet name="CRM" sheetId="2" r:id="rId2"/>
+    <sheet name="GOOG" sheetId="3" r:id="rId3"/>
+    <sheet name="WRBY" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="36">
   <si>
-    <t>Valuation of Five9, Inc. on 2022-01-16</t>
+    <t>Valuation of Asana, Inc. on 2022-01-16</t>
   </si>
   <si>
     <t>Year Ended</t>
@@ -117,10 +118,13 @@
     <t>--</t>
   </si>
   <si>
-    <t>Valuation of Asana, Inc. on 2022-01-16</t>
+    <t>Valuation of Salesforce.com Inc on 2022-01-16</t>
   </si>
   <si>
-    <t>Valuation of Open Lending Corporation on 2022-01-16</t>
+    <t>Valuation of Alphabet Inc. on 2022-01-16</t>
+  </si>
+  <si>
+    <t>Valuation of Warby Parker Inc. on 2022-01-16</t>
   </si>
 </sst>
 </file>
@@ -831,7 +835,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <tabColor rgb="FFE11100"/>
+    <tabColor rgb="FFE19800"/>
   </sheetPr>
   <dimension ref="A1:O33"/>
   <sheetViews>
@@ -885,42 +889,42 @@
         <v>1</v>
       </c>
       <c r="B4" s="5">
-        <v>44469</v>
+        <v>44500</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="7">
-        <v>44834</v>
+        <v>44865</v>
       </c>
       <c r="E4" s="4">
-        <v>45199</v>
+        <v>45230</v>
       </c>
       <c r="F4" s="4">
-        <v>45565</v>
+        <v>45596</v>
       </c>
       <c r="G4" s="4">
-        <v>45930</v>
+        <v>45961</v>
       </c>
       <c r="H4" s="4">
-        <v>46295</v>
+        <v>46326</v>
       </c>
       <c r="I4" s="4">
-        <v>46660</v>
+        <v>46691</v>
       </c>
       <c r="J4" s="4">
-        <v>47026</v>
+        <v>47057</v>
       </c>
       <c r="K4" s="4">
-        <v>47391</v>
+        <v>47422</v>
       </c>
       <c r="L4" s="4">
-        <v>47756</v>
+        <v>47787</v>
       </c>
       <c r="M4" s="8">
-        <v>48121</v>
+        <v>48152</v>
       </c>
       <c r="N4" s="6"/>
       <c r="O4" s="5">
-        <v>48487</v>
+        <v>48518</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -928,38 +932,38 @@
         <v>5</v>
       </c>
       <c r="B5" s="10">
-        <v>0.376</v>
+        <v>0.703</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="11">
-        <v>0.3069545673740838</v>
+        <v>0.5610999999999999</v>
       </c>
       <c r="E5" s="12">
-        <v>0.3069545673740838</v>
+        <v>0.5610999999999999</v>
       </c>
       <c r="F5" s="12">
-        <v>0.3069545673740838</v>
+        <v>0.5610999999999999</v>
       </c>
       <c r="G5" s="12">
-        <v>0.3069545673740838</v>
+        <v>0.5610999999999999</v>
       </c>
       <c r="H5" s="12">
-        <v>0.3069545673740838</v>
+        <v>0.5610999999999999</v>
       </c>
       <c r="I5" s="12">
-        <v>0.2586471396450699</v>
+        <v>0.4704350001666666</v>
       </c>
       <c r="J5" s="12">
-        <v>0.2103397119160559</v>
+        <v>0.3797700003333333</v>
       </c>
       <c r="K5" s="12">
-        <v>0.1620322841870419</v>
+        <v>0.2891050005</v>
       </c>
       <c r="L5" s="12">
-        <v>0.1137248564580279</v>
+        <v>0.1984400006666667</v>
       </c>
       <c r="M5" s="13">
-        <v>0.06541742872901396</v>
+        <v>0.1077750008333334</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="10">
@@ -971,42 +975,42 @@
         <v>6</v>
       </c>
       <c r="B6" s="15">
-        <v>563877000</v>
+        <v>334857000</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="16">
-        <v>736961620.5871964</v>
+        <v>522745262.7</v>
       </c>
       <c r="E6" s="17">
-        <v>963175356.0058429</v>
+        <v>816057629.6009699</v>
       </c>
       <c r="F6" s="17">
-        <v>1258826430.713996</v>
+        <v>1273947565.570074</v>
       </c>
       <c r="G6" s="17">
-        <v>1645228953.152872</v>
+        <v>1988759544.611443</v>
       </c>
       <c r="H6" s="17">
-        <v>2150239494.699229</v>
+        <v>3104652525.092923</v>
       </c>
       <c r="I6" s="17">
-        <v>2706392789.555045</v>
+        <v>4565189736.252454</v>
       </c>
       <c r="J6" s="17">
-        <v>3275654669.241745</v>
+        <v>6298911843.910778</v>
       </c>
       <c r="K6" s="17">
-        <v>3806416477.506933</v>
+        <v>8119958755.694059</v>
       </c>
       <c r="L6" s="17">
-        <v>4239300645.030882</v>
+        <v>9731283376.587294</v>
       </c>
       <c r="M6" s="18">
-        <v>4516624792.838052</v>
+        <v>10780072450.60839</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="15">
-        <v>4593904247.560136</v>
+        <v>10964519501.01838</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1014,42 +1018,42 @@
         <v>7</v>
       </c>
       <c r="B7" s="10">
-        <v>-0.04565889369490155</v>
+        <v>-0.6841278515903804</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="11">
-        <v>-0.01746662316705846</v>
+        <v>-0.5938422012470048</v>
       </c>
       <c r="E7" s="12">
-        <v>0.01072564736078462</v>
+        <v>-0.5035565509036292</v>
       </c>
       <c r="F7" s="12">
-        <v>0.03891791788862771</v>
+        <v>-0.4132709005602536</v>
       </c>
       <c r="G7" s="12">
-        <v>0.06711018841647079</v>
+        <v>-0.322985250216878</v>
       </c>
       <c r="H7" s="12">
-        <v>0.09530245894431387</v>
+        <v>-0.2326995998735024</v>
       </c>
       <c r="I7" s="12">
-        <v>0.123494729472157</v>
+        <v>-0.1424139495301268</v>
       </c>
       <c r="J7" s="12">
-        <v>0.151687</v>
+        <v>-0.0521282991867511</v>
       </c>
       <c r="K7" s="12">
-        <v>0.151687</v>
+        <v>0.03815735115662444</v>
       </c>
       <c r="L7" s="12">
-        <v>0.151687</v>
+        <v>0.1284430015</v>
       </c>
       <c r="M7" s="13">
-        <v>0.151687</v>
+        <v>0.1284430015</v>
       </c>
       <c r="N7" s="6"/>
       <c r="O7" s="10">
-        <v>0.151687</v>
+        <v>0.1284430015</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1057,42 +1061,42 @@
         <v>8</v>
       </c>
       <c r="B8" s="15">
-        <v>-25746000</v>
+        <v>-229085000</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="16">
-        <v>-12872230.91538127</v>
+        <v>-310428197.4932118</v>
       </c>
       <c r="E8" s="17">
-        <v>10330679.21511686</v>
+        <v>-410931165.3004557</v>
       </c>
       <c r="F8" s="17">
-        <v>48990903.66656158</v>
+        <v>-526485457.6896872</v>
       </c>
       <c r="G8" s="17">
-        <v>110411625.0343223</v>
+        <v>-642339999.137531</v>
       </c>
       <c r="H8" s="17">
-        <v>204923111.1640155</v>
+        <v>-722451400.3353819</v>
       </c>
       <c r="I8" s="17">
-        <v>334225245.3914965</v>
+        <v>-650146700.6941097</v>
       </c>
       <c r="J8" s="17">
-        <v>496874229.8132725</v>
+        <v>-328351561.1503511</v>
       </c>
       <c r="K8" s="17">
-        <v>577383896.2235942</v>
+        <v>309836117.6183255</v>
       </c>
       <c r="L8" s="17">
-        <v>643046796.9427994</v>
+        <v>1249915245.335927</v>
       </c>
       <c r="M8" s="18">
-        <v>685113264.9512256</v>
+        <v>1384624861.943602</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="15">
-        <v>696835553.5996544</v>
+        <v>1408315794.716082</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1104,38 +1108,38 @@
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="20">
-        <v>25746000</v>
+        <v>229085000</v>
       </c>
       <c r="E9" s="21">
-        <v>38618230.91538127</v>
+        <v>539513197.4932117</v>
       </c>
       <c r="F9" s="21">
-        <v>28287551.70026441</v>
+        <v>950444362.7936676</v>
       </c>
       <c r="G9" s="21">
-        <v>0</v>
+        <v>1476929820.483355</v>
       </c>
       <c r="H9" s="21">
-        <v>0</v>
+        <v>2119269819.620886</v>
       </c>
       <c r="I9" s="21">
-        <v>0</v>
+        <v>2841721219.956268</v>
       </c>
       <c r="J9" s="21">
-        <v>0</v>
+        <v>3491867920.650377</v>
       </c>
       <c r="K9" s="21">
-        <v>0</v>
+        <v>3820219481.800728</v>
       </c>
       <c r="L9" s="21">
-        <v>0</v>
+        <v>3510383364.182403</v>
       </c>
       <c r="M9" s="22">
-        <v>0</v>
+        <v>2260468118.846476</v>
       </c>
       <c r="N9" s="6"/>
       <c r="O9" s="19">
-        <v>0</v>
+        <v>875843256.9028733</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1153,32 +1157,32 @@
         <v>0</v>
       </c>
       <c r="F10" s="21">
-        <v>20703351.96629717</v>
+        <v>0</v>
       </c>
       <c r="G10" s="21">
-        <v>110411625.0343223</v>
+        <v>0</v>
       </c>
       <c r="H10" s="21">
-        <v>204923111.1640155</v>
+        <v>0</v>
       </c>
       <c r="I10" s="21">
-        <v>334225245.3914965</v>
+        <v>0</v>
       </c>
       <c r="J10" s="21">
-        <v>496874229.8132725</v>
+        <v>0</v>
       </c>
       <c r="K10" s="21">
-        <v>577383896.2235942</v>
+        <v>0</v>
       </c>
       <c r="L10" s="21">
-        <v>643046796.9427994</v>
+        <v>0</v>
       </c>
       <c r="M10" s="22">
-        <v>685113264.9512256</v>
+        <v>0</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="19">
-        <v>696835553.5996544</v>
+        <v>532472537.8132091</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1229,42 +1233,42 @@
         <v>12</v>
       </c>
       <c r="B12" s="15">
-        <v>-25746000</v>
+        <v>-229085000</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="16">
-        <v>-12872230.91538127</v>
+        <v>-310428197.4932118</v>
       </c>
       <c r="E12" s="17">
-        <v>10330679.21511686</v>
+        <v>-410931165.3004557</v>
       </c>
       <c r="F12" s="17">
-        <v>44022099.19465026</v>
+        <v>-526485457.6896872</v>
       </c>
       <c r="G12" s="17">
-        <v>83912835.02608491</v>
+        <v>-642339999.137531</v>
       </c>
       <c r="H12" s="17">
-        <v>155741564.4846518</v>
+        <v>-722451400.3353819</v>
       </c>
       <c r="I12" s="17">
-        <v>254011186.4975374</v>
+        <v>-650146700.6941097</v>
       </c>
       <c r="J12" s="17">
-        <v>377624414.6580871</v>
+        <v>-328351561.1503511</v>
       </c>
       <c r="K12" s="17">
-        <v>438811761.1299316</v>
+        <v>309836117.6183255</v>
       </c>
       <c r="L12" s="17">
-        <v>488715565.6765276</v>
+        <v>1249915245.335927</v>
       </c>
       <c r="M12" s="18">
-        <v>520686081.3629315</v>
+        <v>1384624861.943602</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="15">
-        <v>529595020.7357374</v>
+        <v>1280522385.640912</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1272,42 +1276,42 @@
         <v>13</v>
       </c>
       <c r="B13" s="10">
-        <v>1.165531633163106</v>
+        <v>1.26193609101156</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="11">
-        <v>1.165531633163106</v>
+        <v>1.26193609101156</v>
       </c>
       <c r="E13" s="12">
-        <v>1.165531633163106</v>
+        <v>1.26193609101156</v>
       </c>
       <c r="F13" s="12">
-        <v>1.165531633163106</v>
+        <v>1.26193609101156</v>
       </c>
       <c r="G13" s="12">
-        <v>1.165531633163106</v>
+        <v>1.26193609101156</v>
       </c>
       <c r="H13" s="12">
-        <v>1.165531633163106</v>
+        <v>1.26193609101156</v>
       </c>
       <c r="I13" s="12">
-        <v>1.165531633163106</v>
+        <v>1.26193609101156</v>
       </c>
       <c r="J13" s="12">
-        <v>1.165531633163106</v>
+        <v>1.26193609101156</v>
       </c>
       <c r="K13" s="12">
-        <v>1.165531633163106</v>
+        <v>1.26193609101156</v>
       </c>
       <c r="L13" s="12">
-        <v>1.165531633163106</v>
+        <v>1.26193609101156</v>
       </c>
       <c r="M13" s="13">
-        <v>1.165531633163106</v>
+        <v>1.26193609101156</v>
       </c>
       <c r="N13" s="6"/>
       <c r="O13" s="10">
-        <v>1.165531633163106</v>
+        <v>1.26193609101156</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -1319,38 +1323,38 @@
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="20">
-        <v>148502722.4164363</v>
+        <v>148888889.0953186</v>
       </c>
       <c r="E14" s="21">
-        <v>194086311.329647</v>
+        <v>232430444.7667018</v>
       </c>
       <c r="F14" s="21">
-        <v>253661991.0570707</v>
+        <v>362847167.3252981</v>
       </c>
       <c r="G14" s="21">
-        <v>331524697.7812424</v>
+        <v>566440712.9115229</v>
       </c>
       <c r="H14" s="21">
-        <v>433287717.9625077</v>
+        <v>884270596.9261782</v>
       </c>
       <c r="I14" s="21">
-        <v>477167053.2411771</v>
+        <v>1157378112.538785</v>
       </c>
       <c r="J14" s="21">
-        <v>488413925.0187439</v>
+        <v>1373858882.400759</v>
       </c>
       <c r="K14" s="21">
-        <v>455381727.2421582</v>
+        <v>1443057952.581055</v>
       </c>
       <c r="L14" s="21">
-        <v>371404906.7455643</v>
+        <v>1276867055.606284</v>
       </c>
       <c r="M14" s="22">
-        <v>237937898.8235155</v>
+        <v>831095236.5110632</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="19">
-        <v>66304038.88083015</v>
+        <v>146161958.3778851</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1362,38 +1366,38 @@
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="16">
-        <v>-161374953.3318175</v>
+        <v>-459317086.5885304</v>
       </c>
       <c r="E15" s="17">
-        <v>-183755632.1145302</v>
+        <v>-643361610.0671575</v>
       </c>
       <c r="F15" s="17">
-        <v>-209639891.8624204</v>
+        <v>-889332625.0149853</v>
       </c>
       <c r="G15" s="17">
-        <v>-247611862.7551575</v>
+        <v>-1208780712.049054</v>
       </c>
       <c r="H15" s="17">
-        <v>-277546153.4778559</v>
+        <v>-1606721997.26156</v>
       </c>
       <c r="I15" s="17">
-        <v>-223155866.7436397</v>
+        <v>-1807524813.232894</v>
       </c>
       <c r="J15" s="17">
-        <v>-110789510.3606567</v>
+        <v>-1702210443.55111</v>
       </c>
       <c r="K15" s="17">
-        <v>-16569966.11222661</v>
+        <v>-1133221834.962729</v>
       </c>
       <c r="L15" s="17">
-        <v>117310658.9309633</v>
+        <v>-26951810.27035713</v>
       </c>
       <c r="M15" s="18">
-        <v>282748182.539416</v>
+        <v>553529625.4325391</v>
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="15">
-        <v>463290981.8549072</v>
+        <v>1134360427.263027</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1405,38 +1409,38 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="11">
-        <v>0.072273346587495</v>
+        <v>0.07514240345993498</v>
       </c>
       <c r="E16" s="12">
-        <v>0.072273346587495</v>
+        <v>0.07514240345993498</v>
       </c>
       <c r="F16" s="12">
-        <v>0.072273346587495</v>
+        <v>0.07514240345993498</v>
       </c>
       <c r="G16" s="12">
-        <v>0.072273346587495</v>
+        <v>0.07514240345993498</v>
       </c>
       <c r="H16" s="12">
-        <v>0.072273346587495</v>
+        <v>0.07514240345993498</v>
       </c>
       <c r="I16" s="12">
-        <v>0.07142640112187042</v>
+        <v>0.07405636992160707</v>
       </c>
       <c r="J16" s="12">
-        <v>0.07057945565624583</v>
+        <v>0.07297033638327914</v>
       </c>
       <c r="K16" s="12">
-        <v>0.06973251019062124</v>
+        <v>0.07188430284495123</v>
       </c>
       <c r="L16" s="12">
-        <v>0.06888556472499666</v>
+        <v>0.07079826930662332</v>
       </c>
       <c r="M16" s="13">
-        <v>0.06803861925937207</v>
+        <v>0.0697122357682954</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="10">
-        <v>0.06719167379374749</v>
+        <v>0.06862620222996749</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1448,34 +1452,34 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="11">
-        <v>0.932598020068759</v>
+        <v>0.9301093481029881</v>
       </c>
       <c r="E17" s="12">
-        <v>0.8697390670361694</v>
+        <v>0.8651033994285654</v>
       </c>
       <c r="F17" s="12">
-        <v>0.8111169318943813</v>
+        <v>0.8046407588841819</v>
       </c>
       <c r="G17" s="12">
-        <v>0.7564460447289464</v>
+        <v>0.74840389170286</v>
       </c>
       <c r="H17" s="12">
-        <v>0.7054600836030593</v>
+        <v>0.6960974558294865</v>
       </c>
       <c r="I17" s="12">
-        <v>0.6584307450930698</v>
+        <v>0.6481014175078101</v>
       </c>
       <c r="J17" s="12">
-        <v>0.6150227725876392</v>
+        <v>0.6040254753849036</v>
       </c>
       <c r="K17" s="12">
-        <v>0.5749313652980829</v>
+        <v>0.5635174186073292</v>
       </c>
       <c r="L17" s="12">
-        <v>0.537879249446129</v>
+        <v>0.5262591794925341</v>
       </c>
       <c r="M17" s="13">
-        <v>0.5036140451729354</v>
+        <v>0.491963316764869</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="10" t="s">
@@ -1491,38 +1495,38 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="16">
-        <v>-150497961.9659414</v>
+        <v>-427215115.9794217</v>
       </c>
       <c r="E18" s="17">
-        <v>-159819452.0379331</v>
+        <v>-556574315.9309331</v>
       </c>
       <c r="F18" s="17">
-        <v>-170042465.8901163</v>
+        <v>-715593278.2925193</v>
       </c>
       <c r="G18" s="17">
-        <v>-187305014.2091056</v>
+        <v>-904656189.1128662</v>
       </c>
       <c r="H18" s="17">
-        <v>-195797732.6361958</v>
+        <v>-1118435094.519043</v>
       </c>
       <c r="I18" s="17">
-        <v>-146932683.6119045</v>
+        <v>-1171459393.636779</v>
       </c>
       <c r="J18" s="17">
-        <v>-68138071.83563808</v>
+        <v>-1028178472.371107</v>
       </c>
       <c r="K18" s="17">
-        <v>-9526593.239845408</v>
+        <v>-638590243.147658</v>
       </c>
       <c r="L18" s="17">
-        <v>63098969.17781739</v>
+        <v>-14183637.5587166</v>
       </c>
       <c r="M18" s="18">
-        <v>142395955.9739708</v>
+        <v>272316270.4554075</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="15">
-        <v>4658786986.30889</v>
+        <v>10832780851.05587</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1535,7 +1539,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="19">
-        <v>-882565050.2748922</v>
+        <v>-6302569470.093637</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1543,7 +1547,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="19">
-        <v>4658786986.30889</v>
+        <v>10832780851.05587</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1551,7 +1555,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="15">
-        <v>3776221936.033998</v>
+        <v>4530211380.962234</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1559,7 +1563,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="19">
-        <v>827345984</v>
+        <v>255090000</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -1575,7 +1579,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="19">
-        <v>415288992</v>
+        <v>343396000</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -1591,7 +1595,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="15">
-        <v>3364164944.033998</v>
+        <v>4618517380.962234</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -1599,7 +1603,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="19">
-        <v>8734770176</v>
+        <v>11219297280</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -1607,7 +1611,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="19">
-        <v>68049000</v>
+        <v>97690400</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -1615,7 +1619,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="25">
-        <v>49.43738988132078</v>
+        <v>47.27708537340654</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -1623,7 +1627,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="27">
-        <v>128.36</v>
+        <v>60.18</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1631,7 +1635,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="29">
-        <v>0.3851463842421375</v>
+        <v>0.7855946389731894</v>
       </c>
     </row>
   </sheetData>
@@ -1642,7 +1646,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <tabColor rgb="FFE19800"/>
+    <tabColor rgb="FFE10000"/>
   </sheetPr>
   <dimension ref="A1:O33"/>
   <sheetViews>
@@ -1739,38 +1743,38 @@
         <v>5</v>
       </c>
       <c r="B5" s="10">
-        <v>0.703</v>
+        <v>0.266</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="11">
-        <v>0.5610999999999999</v>
+        <v>0.2546410854503579</v>
       </c>
       <c r="E5" s="12">
-        <v>0.5610999999999999</v>
+        <v>0.2546410854503579</v>
       </c>
       <c r="F5" s="12">
-        <v>0.5610999999999999</v>
+        <v>0.2546410854503579</v>
       </c>
       <c r="G5" s="12">
-        <v>0.5610999999999999</v>
+        <v>0.2546410854503579</v>
       </c>
       <c r="H5" s="12">
-        <v>0.5610999999999999</v>
+        <v>0.2546410854503579</v>
       </c>
       <c r="I5" s="12">
-        <v>0.4704350001666666</v>
+        <v>0.2150525713752983</v>
       </c>
       <c r="J5" s="12">
-        <v>0.3797700003333333</v>
+        <v>0.1754640573002386</v>
       </c>
       <c r="K5" s="12">
-        <v>0.2891050005</v>
+        <v>0.1358755432251789</v>
       </c>
       <c r="L5" s="12">
-        <v>0.1984400006666667</v>
+        <v>0.0962870291501193</v>
       </c>
       <c r="M5" s="13">
-        <v>0.1077750008333334</v>
+        <v>0.05669851507505966</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="10">
@@ -1782,42 +1786,42 @@
         <v>6</v>
       </c>
       <c r="B6" s="15">
-        <v>334857000</v>
+        <v>24983000000</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="16">
-        <v>522745262.7</v>
+        <v>31344698237.80629</v>
       </c>
       <c r="E6" s="17">
-        <v>816057629.6009699</v>
+        <v>39326346220.1952</v>
       </c>
       <c r="F6" s="17">
-        <v>1273947565.570074</v>
+        <v>49340449708.50228</v>
       </c>
       <c r="G6" s="17">
-        <v>1988759544.611443</v>
+        <v>61904555378.88409</v>
       </c>
       <c r="H6" s="17">
-        <v>3104652525.092923</v>
+        <v>77667998554.88492</v>
       </c>
       <c r="I6" s="17">
-        <v>4565189736.252454</v>
+        <v>94370701357.68587</v>
       </c>
       <c r="J6" s="17">
-        <v>6298911843.910778</v>
+        <v>110929367508.1746</v>
       </c>
       <c r="K6" s="17">
-        <v>8119958755.694059</v>
+        <v>126001955577.9733</v>
       </c>
       <c r="L6" s="17">
-        <v>9731283376.587294</v>
+        <v>138134309547.6816</v>
       </c>
       <c r="M6" s="18">
-        <v>10780072450.60839</v>
+        <v>145966319779.9538</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="15">
-        <v>10964519501.01838</v>
+        <v>148463803657.3552</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1825,32 +1829,32 @@
         <v>7</v>
       </c>
       <c r="B7" s="10">
-        <v>-0.6841278515903804</v>
+        <v>0.03886642917183685</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="11">
-        <v>-0.5938422012470048</v>
+        <v>0.05379585789319737</v>
       </c>
       <c r="E7" s="12">
-        <v>-0.5035565509036292</v>
+        <v>0.0687252866145579</v>
       </c>
       <c r="F7" s="12">
-        <v>-0.4132709005602536</v>
+        <v>0.08365471533591842</v>
       </c>
       <c r="G7" s="12">
-        <v>-0.322985250216878</v>
+        <v>0.09858414405727894</v>
       </c>
       <c r="H7" s="12">
-        <v>-0.2326995998735024</v>
+        <v>0.1135135727786395</v>
       </c>
       <c r="I7" s="12">
-        <v>-0.1424139495301268</v>
+        <v>0.1284430015</v>
       </c>
       <c r="J7" s="12">
-        <v>-0.0521282991867511</v>
+        <v>0.1284430015</v>
       </c>
       <c r="K7" s="12">
-        <v>0.03815735115662444</v>
+        <v>0.1284430015</v>
       </c>
       <c r="L7" s="12">
         <v>0.1284430015</v>
@@ -1868,42 +1872,42 @@
         <v>8</v>
       </c>
       <c r="B8" s="15">
-        <v>-229085000</v>
+        <v>971000000</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="16">
-        <v>-310428197.4932118</v>
+        <v>1686214932.106181</v>
       </c>
       <c r="E8" s="17">
-        <v>-410931165.3004557</v>
+        <v>2702714415.486251</v>
       </c>
       <c r="F8" s="17">
-        <v>-526485457.6896872</v>
+        <v>4127561274.910957</v>
       </c>
       <c r="G8" s="17">
-        <v>-642339999.137531</v>
+        <v>6102807605.273711</v>
       </c>
       <c r="H8" s="17">
-        <v>-722451400.3353819</v>
+        <v>8816372006.531195</v>
       </c>
       <c r="I8" s="17">
-        <v>-650146700.6941097</v>
+        <v>12121256136.0413</v>
       </c>
       <c r="J8" s="17">
-        <v>-328351561.1503511</v>
+        <v>14248100917.24652</v>
       </c>
       <c r="K8" s="17">
-        <v>309836117.6183255</v>
+        <v>16184069369.30456</v>
       </c>
       <c r="L8" s="17">
-        <v>1249915245.335927</v>
+        <v>17742385328.43433</v>
       </c>
       <c r="M8" s="18">
-        <v>1384624861.943602</v>
+        <v>18748352230.44609</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="15">
-        <v>1408315794.716082</v>
+        <v>19069136555.85737</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1915,38 +1919,38 @@
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="20">
-        <v>229085000</v>
+        <v>0</v>
       </c>
       <c r="E9" s="21">
-        <v>539513197.4932117</v>
+        <v>0</v>
       </c>
       <c r="F9" s="21">
-        <v>950444362.7936676</v>
+        <v>0</v>
       </c>
       <c r="G9" s="21">
-        <v>1476929820.483355</v>
+        <v>0</v>
       </c>
       <c r="H9" s="21">
-        <v>2119269819.620886</v>
+        <v>0</v>
       </c>
       <c r="I9" s="21">
-        <v>2841721219.956268</v>
+        <v>0</v>
       </c>
       <c r="J9" s="21">
-        <v>3491867920.650377</v>
+        <v>0</v>
       </c>
       <c r="K9" s="21">
-        <v>3820219481.800728</v>
+        <v>0</v>
       </c>
       <c r="L9" s="21">
-        <v>3510383364.182403</v>
+        <v>0</v>
       </c>
       <c r="M9" s="22">
-        <v>2260468118.846476</v>
+        <v>0</v>
       </c>
       <c r="N9" s="6"/>
       <c r="O9" s="19">
-        <v>875843256.9028733</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1954,42 +1958,42 @@
         <v>10</v>
       </c>
       <c r="B10" s="19">
-        <v>0</v>
+        <v>971000000</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="20">
-        <v>0</v>
+        <v>1686214932.106181</v>
       </c>
       <c r="E10" s="21">
-        <v>0</v>
+        <v>2702714415.486251</v>
       </c>
       <c r="F10" s="21">
-        <v>0</v>
+        <v>4127561274.910957</v>
       </c>
       <c r="G10" s="21">
-        <v>0</v>
+        <v>6102807605.273711</v>
       </c>
       <c r="H10" s="21">
-        <v>0</v>
+        <v>8816372006.531195</v>
       </c>
       <c r="I10" s="21">
-        <v>0</v>
+        <v>12121256136.0413</v>
       </c>
       <c r="J10" s="21">
-        <v>0</v>
+        <v>14248100917.24652</v>
       </c>
       <c r="K10" s="21">
-        <v>0</v>
+        <v>16184069369.30456</v>
       </c>
       <c r="L10" s="21">
-        <v>0</v>
+        <v>17742385328.43433</v>
       </c>
       <c r="M10" s="22">
-        <v>0</v>
+        <v>18748352230.44609</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="19">
-        <v>532472537.8132091</v>
+        <v>19069136555.85737</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -2040,42 +2044,42 @@
         <v>12</v>
       </c>
       <c r="B12" s="15">
-        <v>-229085000</v>
+        <v>737960000</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="16">
-        <v>-310428197.4932118</v>
+        <v>1281523348.400698</v>
       </c>
       <c r="E12" s="17">
-        <v>-410931165.3004557</v>
+        <v>2054062955.769551</v>
       </c>
       <c r="F12" s="17">
-        <v>-526485457.6896872</v>
+        <v>3136946568.932328</v>
       </c>
       <c r="G12" s="17">
-        <v>-642339999.137531</v>
+        <v>4638133780.00802</v>
       </c>
       <c r="H12" s="17">
-        <v>-722451400.3353819</v>
+        <v>6700442724.963708</v>
       </c>
       <c r="I12" s="17">
-        <v>-650146700.6941097</v>
+        <v>9212154663.391384</v>
       </c>
       <c r="J12" s="17">
-        <v>-328351561.1503511</v>
+        <v>10828556697.10735</v>
       </c>
       <c r="K12" s="17">
-        <v>309836117.6183255</v>
+        <v>12299892720.67146</v>
       </c>
       <c r="L12" s="17">
-        <v>1249915245.335927</v>
+        <v>13484212849.61009</v>
       </c>
       <c r="M12" s="18">
-        <v>1384624861.943602</v>
+        <v>14248747695.13903</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="15">
-        <v>1280522385.640912</v>
+        <v>14492543782.4516</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -2083,42 +2087,42 @@
         <v>13</v>
       </c>
       <c r="B13" s="10">
-        <v>1.26193609101156</v>
+        <v>0.8626844115109444</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="11">
-        <v>1.26193609101156</v>
+        <v>0.8626844115109444</v>
       </c>
       <c r="E13" s="12">
-        <v>1.26193609101156</v>
+        <v>0.8626844115109444</v>
       </c>
       <c r="F13" s="12">
-        <v>1.26193609101156</v>
+        <v>0.8626844115109444</v>
       </c>
       <c r="G13" s="12">
-        <v>1.26193609101156</v>
+        <v>0.8626844115109444</v>
       </c>
       <c r="H13" s="12">
-        <v>1.26193609101156</v>
+        <v>0.8626844115109444</v>
       </c>
       <c r="I13" s="12">
-        <v>1.26193609101156</v>
+        <v>0.8626844115109444</v>
       </c>
       <c r="J13" s="12">
-        <v>1.26193609101156</v>
+        <v>0.8626844115109444</v>
       </c>
       <c r="K13" s="12">
-        <v>1.26193609101156</v>
+        <v>0.8626844115109444</v>
       </c>
       <c r="L13" s="12">
-        <v>1.26193609101156</v>
+        <v>0.8626844115109444</v>
       </c>
       <c r="M13" s="13">
-        <v>1.26193609101156</v>
+        <v>0.8626844115109444</v>
       </c>
       <c r="N13" s="6"/>
       <c r="O13" s="10">
-        <v>1.26193609101156</v>
+        <v>0.8626844115109444</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -2130,38 +2134,38 @@
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="20">
-        <v>148888889.0953186</v>
+        <v>7374305311.329463</v>
       </c>
       <c r="E14" s="21">
-        <v>232430444.7667018</v>
+        <v>9252106420.248732</v>
       </c>
       <c r="F14" s="21">
-        <v>362847167.3252981</v>
+        <v>11608072841.8031</v>
       </c>
       <c r="G14" s="21">
-        <v>566440712.9115229</v>
+        <v>14563965110.22666</v>
       </c>
       <c r="H14" s="21">
-        <v>884270596.9261782</v>
+        <v>18272548994.35591</v>
       </c>
       <c r="I14" s="21">
-        <v>1157378112.538785</v>
+        <v>19361312874.01737</v>
       </c>
       <c r="J14" s="21">
-        <v>1373858882.400759</v>
+        <v>19194349555.34562</v>
       </c>
       <c r="K14" s="21">
-        <v>1443057952.581055</v>
+        <v>17471728790.60133</v>
       </c>
       <c r="L14" s="21">
-        <v>1276867055.606284</v>
+        <v>14063490435.00066</v>
       </c>
       <c r="M14" s="22">
-        <v>831095236.5110632</v>
+        <v>9078650463.330906</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="19">
-        <v>146161958.3778851</v>
+        <v>2895014496.700051</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -2173,38 +2177,38 @@
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="16">
-        <v>-459317086.5885304</v>
+        <v>-6092781962.928765</v>
       </c>
       <c r="E15" s="17">
-        <v>-643361610.0671575</v>
+        <v>-7198043464.479181</v>
       </c>
       <c r="F15" s="17">
-        <v>-889332625.0149853</v>
+        <v>-8471126272.870771</v>
       </c>
       <c r="G15" s="17">
-        <v>-1208780712.049054</v>
+        <v>-9925831330.218639</v>
       </c>
       <c r="H15" s="17">
-        <v>-1606721997.26156</v>
+        <v>-11572106269.3922</v>
       </c>
       <c r="I15" s="17">
-        <v>-1807524813.232894</v>
+        <v>-10149158210.62599</v>
       </c>
       <c r="J15" s="17">
-        <v>-1702210443.55111</v>
+        <v>-8365792858.238268</v>
       </c>
       <c r="K15" s="17">
-        <v>-1133221834.962729</v>
+        <v>-5171836069.929871</v>
       </c>
       <c r="L15" s="17">
-        <v>-26951810.27035713</v>
+        <v>-579277585.3905697</v>
       </c>
       <c r="M15" s="18">
-        <v>553529625.4325391</v>
+        <v>5170097231.808121</v>
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="15">
-        <v>1134360427.263027</v>
+        <v>11597529285.75155</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -2216,38 +2220,38 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="11">
-        <v>0.07514240345993498</v>
+        <v>0.07486139272426998</v>
       </c>
       <c r="E16" s="12">
-        <v>0.07514240345993498</v>
+        <v>0.07486139272426998</v>
       </c>
       <c r="F16" s="12">
-        <v>0.07514240345993498</v>
+        <v>0.07486139272426998</v>
       </c>
       <c r="G16" s="12">
-        <v>0.07514240345993498</v>
+        <v>0.07486139272426998</v>
       </c>
       <c r="H16" s="12">
-        <v>0.07514240345993498</v>
+        <v>0.07486139272426998</v>
       </c>
       <c r="I16" s="12">
-        <v>0.07405636992160707</v>
+        <v>0.07379877674724748</v>
       </c>
       <c r="J16" s="12">
-        <v>0.07297033638327914</v>
+        <v>0.07273616077022498</v>
       </c>
       <c r="K16" s="12">
-        <v>0.07188430284495123</v>
+        <v>0.07167354479320248</v>
       </c>
       <c r="L16" s="12">
-        <v>0.07079826930662332</v>
+        <v>0.07061092881617999</v>
       </c>
       <c r="M16" s="13">
-        <v>0.0697122357682954</v>
+        <v>0.06954831283915748</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="10">
-        <v>0.06862620222996749</v>
+        <v>0.06848569686213499</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -2259,34 +2263,34 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="11">
-        <v>0.9301093481029881</v>
+        <v>0.9303525150023935</v>
       </c>
       <c r="E17" s="12">
-        <v>0.8651033994285654</v>
+        <v>0.8655558021712788</v>
       </c>
       <c r="F17" s="12">
-        <v>0.8046407588841819</v>
+        <v>0.8052720174249633</v>
       </c>
       <c r="G17" s="12">
-        <v>0.74840389170286</v>
+        <v>0.7491868466723659</v>
       </c>
       <c r="H17" s="12">
-        <v>0.6960974558294865</v>
+        <v>0.6970078670083482</v>
       </c>
       <c r="I17" s="12">
-        <v>0.6481014175078101</v>
+        <v>0.6491047318192382</v>
       </c>
       <c r="J17" s="12">
-        <v>0.6040254753849036</v>
+        <v>0.6050926178839545</v>
       </c>
       <c r="K17" s="12">
-        <v>0.5635174186073292</v>
+        <v>0.5646240133703379</v>
       </c>
       <c r="L17" s="12">
-        <v>0.5262591794925341</v>
+        <v>0.5273848773379014</v>
       </c>
       <c r="M17" s="13">
-        <v>0.491963316764869</v>
+        <v>0.4930912152420098</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="10" t="s">
@@ -2302,38 +2306,38 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="16">
-        <v>-427215115.9794217</v>
+        <v>-5668435022.571997</v>
       </c>
       <c r="E18" s="17">
-        <v>-556574315.9309331</v>
+        <v>-6230308284.961009</v>
       </c>
       <c r="F18" s="17">
-        <v>-715593278.2925193</v>
+        <v>-6821560943.616257</v>
       </c>
       <c r="G18" s="17">
-        <v>-904656189.1128662</v>
+        <v>-7436302274.888277</v>
       </c>
       <c r="H18" s="17">
-        <v>-1118435094.519043</v>
+        <v>-8065849107.622991</v>
       </c>
       <c r="I18" s="17">
-        <v>-1171459393.636779</v>
+        <v>-6587866618.499402</v>
       </c>
       <c r="J18" s="17">
-        <v>-1028178472.371107</v>
+        <v>-5062079501.266284</v>
       </c>
       <c r="K18" s="17">
-        <v>-638590243.147658</v>
+        <v>-2920142838.297279</v>
       </c>
       <c r="L18" s="17">
-        <v>-14183637.5587166</v>
+        <v>-305502238.3158013</v>
       </c>
       <c r="M18" s="18">
-        <v>272316270.4554075</v>
+        <v>2549329526.951617</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="15">
-        <v>10832780851.05587</v>
+        <v>111310216111.9494</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -2346,7 +2350,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="19">
-        <v>-6302569470.093637</v>
+        <v>-46548717303.08768</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -2354,7 +2358,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="19">
-        <v>10832780851.05587</v>
+        <v>111310216111.9494</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -2362,7 +2366,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="15">
-        <v>4530211380.962234</v>
+        <v>64761498808.86175</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -2370,7 +2374,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="19">
-        <v>255090000</v>
+        <v>14337999872</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -2386,7 +2390,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="19">
-        <v>343396000</v>
+        <v>9390999552</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -2402,7 +2406,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="15">
-        <v>4618517380.962234</v>
+        <v>59814498488.86176</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -2410,7 +2414,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="19">
-        <v>11219297280</v>
+        <v>227761553408</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -2418,7 +2422,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="19">
-        <v>97690400</v>
+        <v>985000000</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -2426,7 +2430,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="25">
-        <v>47.27708537340654</v>
+        <v>60.7253791765094</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -2434,7 +2438,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="27">
-        <v>60.18</v>
+        <v>231.23</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -2442,7 +2446,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="29">
-        <v>0.7855946389731894</v>
+        <v>0.2626189472668313</v>
       </c>
     </row>
   </sheetData>
@@ -2550,38 +2554,38 @@
         <v>5</v>
       </c>
       <c r="B5" s="10">
-        <v>0.979</v>
+        <v>0.41</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="11">
-        <v>0.629034354902506</v>
+        <v>0.3201761451922981</v>
       </c>
       <c r="E5" s="12">
-        <v>0.629034354902506</v>
+        <v>0.3201761451922981</v>
       </c>
       <c r="F5" s="12">
-        <v>0.629034354902506</v>
+        <v>0.3201761451922981</v>
       </c>
       <c r="G5" s="12">
-        <v>0.629034354902506</v>
+        <v>0.3201761451922981</v>
       </c>
       <c r="H5" s="12">
-        <v>0.629034354902506</v>
+        <v>0.3201761451922981</v>
       </c>
       <c r="I5" s="12">
-        <v>0.5270469625854217</v>
+        <v>0.2696651211602484</v>
       </c>
       <c r="J5" s="12">
-        <v>0.4250595702683374</v>
+        <v>0.2191540971281987</v>
       </c>
       <c r="K5" s="12">
-        <v>0.323072177951253</v>
+        <v>0.168643073096149</v>
       </c>
       <c r="L5" s="12">
-        <v>0.2210847856341687</v>
+        <v>0.1181320490640994</v>
       </c>
       <c r="M5" s="13">
-        <v>0.1190973933170844</v>
+        <v>0.0676210250320497</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="10">
@@ -2593,42 +2597,42 @@
         <v>6</v>
       </c>
       <c r="B6" s="15">
-        <v>203658000</v>
+        <v>239210000000</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="16">
-        <v>331765878.6507345</v>
+        <v>315799335691.4496</v>
       </c>
       <c r="E6" s="17">
-        <v>540458014.1064624</v>
+        <v>416910749647.4266</v>
       </c>
       <c r="F6" s="17">
-        <v>880424672.3618103</v>
+        <v>550395626358.7709</v>
       </c>
       <c r="G6" s="17">
-        <v>1434242038.181172</v>
+        <v>726619176337.0226</v>
       </c>
       <c r="H6" s="17">
-        <v>2336429553.442521</v>
+        <v>959265303239.4132</v>
       </c>
       <c r="I6" s="17">
-        <v>3567837652.879214</v>
+        <v>1217945697462.292</v>
       </c>
       <c r="J6" s="17">
-        <v>5084381192.399247</v>
+        <v>1484863487140.815</v>
       </c>
       <c r="K6" s="17">
-        <v>6727003297.762061</v>
+        <v>1735275428740.506</v>
       </c>
       <c r="L6" s="17">
-        <v>8214241379.808132</v>
+        <v>1940267070828.205</v>
       </c>
       <c r="M6" s="18">
-        <v>9192536116.22061</v>
+        <v>2071469918993.541</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="15">
-        <v>9349820418.361681</v>
+        <v>2106912771378.991</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -2636,42 +2640,42 @@
         <v>7</v>
       </c>
       <c r="B7" s="10">
-        <v>0.6734820139645877</v>
+        <v>0.302997366330839</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="11">
-        <v>0.6553945250810854</v>
+        <v>0.2887404801286469</v>
       </c>
       <c r="E7" s="12">
-        <v>0.6373070361975831</v>
+        <v>0.2744835939264549</v>
       </c>
       <c r="F7" s="12">
-        <v>0.6192195473140809</v>
+        <v>0.2602267077242629</v>
       </c>
       <c r="G7" s="12">
-        <v>0.6011320584305786</v>
+        <v>0.2459698215220708</v>
       </c>
       <c r="H7" s="12">
-        <v>0.5830445695470763</v>
+        <v>0.2317129353198788</v>
       </c>
       <c r="I7" s="12">
-        <v>0.5830445695470763</v>
+        <v>0.2317129353198788</v>
       </c>
       <c r="J7" s="12">
-        <v>0.5830445695470763</v>
+        <v>0.2317129353198788</v>
       </c>
       <c r="K7" s="12">
-        <v>0.5830445695470763</v>
+        <v>0.2317129353198788</v>
       </c>
       <c r="L7" s="12">
-        <v>0.5830445695470763</v>
+        <v>0.2317129353198788</v>
       </c>
       <c r="M7" s="13">
-        <v>0.5830445695470763</v>
+        <v>0.2317129353198788</v>
       </c>
       <c r="N7" s="6"/>
       <c r="O7" s="10">
-        <v>0.5830445695470763</v>
+        <v>0.2317129353198788</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -2679,42 +2683,42 @@
         <v>8</v>
       </c>
       <c r="B8" s="15">
-        <v>137160000</v>
+        <v>72480000000</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="16">
-        <v>217437540.4764072</v>
+        <v>91184051811.85692</v>
       </c>
       <c r="E8" s="17">
-        <v>344437695.1594211</v>
+        <v>114435160909.7982</v>
       </c>
       <c r="F8" s="17">
-        <v>545176167.0640281</v>
+        <v>143227641793.1765</v>
       </c>
       <c r="G8" s="17">
-        <v>862168868.6995164</v>
+        <v>178726389118.1316</v>
       </c>
       <c r="H8" s="17">
-        <v>1362242563.263962</v>
+        <v>222274179164.1181</v>
       </c>
       <c r="I8" s="17">
-        <v>2080208368.536813</v>
+        <v>282213772619.2047</v>
       </c>
       <c r="J8" s="17">
-        <v>2964420843.73567</v>
+        <v>344062077154.7093</v>
       </c>
       <c r="K8" s="17">
-        <v>3922142742.085443</v>
+        <v>402085763181.9238</v>
       </c>
       <c r="L8" s="17">
-        <v>4789268829.446014</v>
+        <v>449584978286.1066</v>
       </c>
       <c r="M8" s="18">
-        <v>5359658262.927797</v>
+        <v>479986375356.825</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="15">
-        <v>5451362021.166151</v>
+        <v>488198942719.1667</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -2765,42 +2769,42 @@
         <v>10</v>
       </c>
       <c r="B10" s="19">
-        <v>137160000</v>
+        <v>72480000000</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="20">
-        <v>217437540.4764072</v>
+        <v>91184051811.85692</v>
       </c>
       <c r="E10" s="21">
-        <v>344437695.1594211</v>
+        <v>114435160909.7982</v>
       </c>
       <c r="F10" s="21">
-        <v>545176167.0640281</v>
+        <v>143227641793.1765</v>
       </c>
       <c r="G10" s="21">
-        <v>862168868.6995164</v>
+        <v>178726389118.1316</v>
       </c>
       <c r="H10" s="21">
-        <v>1362242563.263962</v>
+        <v>222274179164.1181</v>
       </c>
       <c r="I10" s="21">
-        <v>2080208368.536813</v>
+        <v>282213772619.2047</v>
       </c>
       <c r="J10" s="21">
-        <v>2964420843.73567</v>
+        <v>344062077154.7093</v>
       </c>
       <c r="K10" s="21">
-        <v>3922142742.085443</v>
+        <v>402085763181.9238</v>
       </c>
       <c r="L10" s="21">
-        <v>4789268829.446014</v>
+        <v>449584978286.1066</v>
       </c>
       <c r="M10" s="22">
-        <v>5359658262.927797</v>
+        <v>479986375356.825</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="19">
-        <v>5451362021.166151</v>
+        <v>488198942719.1667</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -2851,42 +2855,42 @@
         <v>12</v>
       </c>
       <c r="B12" s="15">
-        <v>104241600</v>
+        <v>55084800000</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="16">
-        <v>165252530.7620695</v>
+        <v>69299879377.01126</v>
       </c>
       <c r="E12" s="17">
-        <v>261772648.32116</v>
+        <v>86970722291.44659</v>
       </c>
       <c r="F12" s="17">
-        <v>414333886.9686614</v>
+        <v>108853007762.8141</v>
       </c>
       <c r="G12" s="17">
-        <v>655248340.2116325</v>
+        <v>135832055729.78</v>
       </c>
       <c r="H12" s="17">
-        <v>1035304348.080611</v>
+        <v>168928376164.7297</v>
       </c>
       <c r="I12" s="17">
-        <v>1580958360.087977</v>
+        <v>214482467190.5956</v>
       </c>
       <c r="J12" s="17">
-        <v>2252959841.239109</v>
+        <v>261487178637.579</v>
       </c>
       <c r="K12" s="17">
-        <v>2980828483.984937</v>
+        <v>305585180018.2621</v>
       </c>
       <c r="L12" s="17">
-        <v>3639844310.378971</v>
+        <v>341684583497.441</v>
       </c>
       <c r="M12" s="18">
-        <v>4073340279.825126</v>
+        <v>364789645271.187</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="15">
-        <v>4143035136.086275</v>
+        <v>371031196466.5667</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -2894,42 +2898,42 @@
         <v>13</v>
       </c>
       <c r="B13" s="10">
-        <v>0.9277572392489473</v>
+        <v>1.1118661407294</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="11">
-        <v>0.9277572392489473</v>
+        <v>1.1118661407294</v>
       </c>
       <c r="E13" s="12">
-        <v>0.9277572392489473</v>
+        <v>1.1118661407294</v>
       </c>
       <c r="F13" s="12">
-        <v>0.9277572392489473</v>
+        <v>1.1118661407294</v>
       </c>
       <c r="G13" s="12">
-        <v>0.9277572392489473</v>
+        <v>1.1118661407294</v>
       </c>
       <c r="H13" s="12">
-        <v>0.9277572392489473</v>
+        <v>1.1118661407294</v>
       </c>
       <c r="I13" s="12">
-        <v>0.9277572392489473</v>
+        <v>1.1118661407294</v>
       </c>
       <c r="J13" s="12">
-        <v>0.9277572392489473</v>
+        <v>1.1118661407294</v>
       </c>
       <c r="K13" s="12">
-        <v>0.9277572392489473</v>
+        <v>1.1118661407294</v>
       </c>
       <c r="L13" s="12">
-        <v>0.9277572392489473</v>
+        <v>1.1118661407294</v>
       </c>
       <c r="M13" s="13">
-        <v>0.9277572392489473</v>
+        <v>1.1118661407294</v>
       </c>
       <c r="N13" s="6"/>
       <c r="O13" s="10">
-        <v>0.9277572392489473</v>
+        <v>1.1118661407294</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -2941,38 +2945,38 @@
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="20">
-        <v>138083405.0450983</v>
+        <v>68883593884.06767</v>
       </c>
       <c r="E14" s="21">
-        <v>224942610.6603831</v>
+        <v>90938477440.86026</v>
       </c>
       <c r="F14" s="21">
-        <v>366439240.6472227</v>
+        <v>120054808597.5316</v>
       </c>
       <c r="G14" s="21">
-        <v>596942111.9987127</v>
+        <v>158493494426.0885</v>
       </c>
       <c r="H14" s="21">
-        <v>972439208.3339623</v>
+        <v>209239330509.4904</v>
       </c>
       <c r="I14" s="21">
-        <v>1327295597.75094</v>
+        <v>232654260029.162</v>
       </c>
       <c r="J14" s="21">
-        <v>1634634013.470732</v>
+        <v>240062881583.4078</v>
       </c>
       <c r="K14" s="21">
-        <v>1770530086.828075</v>
+        <v>225217706004.9848</v>
       </c>
       <c r="L14" s="21">
-        <v>1603046593.578772</v>
+        <v>184367195455.041</v>
       </c>
       <c r="M14" s="22">
-        <v>1054472759.710765</v>
+        <v>118002377587.7058</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="19">
-        <v>169531743.3129367</v>
+        <v>31876905939.59308</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -2984,38 +2988,38 @@
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="16">
-        <v>27169125.71697119</v>
+        <v>416285492.9435883</v>
       </c>
       <c r="E15" s="17">
-        <v>36830037.66077694</v>
+        <v>-3967755149.413666</v>
       </c>
       <c r="F15" s="17">
-        <v>47894646.32143873</v>
+        <v>-11201800834.7175</v>
       </c>
       <c r="G15" s="17">
-        <v>58306228.21291983</v>
+        <v>-22661438696.30847</v>
       </c>
       <c r="H15" s="17">
-        <v>62865139.74664891</v>
+        <v>-40310954344.76071</v>
       </c>
       <c r="I15" s="17">
-        <v>253662762.3370371</v>
+        <v>-18171792838.56647</v>
       </c>
       <c r="J15" s="17">
-        <v>618325827.7683768</v>
+        <v>21424297054.1712</v>
       </c>
       <c r="K15" s="17">
-        <v>1210298397.156862</v>
+        <v>80367474013.27728</v>
       </c>
       <c r="L15" s="17">
-        <v>2036797716.800199</v>
+        <v>157317388042.4001</v>
       </c>
       <c r="M15" s="18">
-        <v>3018867520.114361</v>
+        <v>246787267683.4812</v>
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="15">
-        <v>3973503392.773338</v>
+        <v>339154290526.9736</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -3027,38 +3031,38 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="11">
-        <v>0.05969448201893227</v>
+        <v>0.0695828499810715</v>
       </c>
       <c r="E16" s="12">
-        <v>0.05969448201893227</v>
+        <v>0.0695828499810715</v>
       </c>
       <c r="F16" s="12">
-        <v>0.05969448201893227</v>
+        <v>0.0695828499810715</v>
       </c>
       <c r="G16" s="12">
-        <v>0.05969448201893227</v>
+        <v>0.0695828499810715</v>
       </c>
       <c r="H16" s="12">
-        <v>0.05969448201893227</v>
+        <v>0.0695828499810715</v>
       </c>
       <c r="I16" s="12">
-        <v>0.05969448201893227</v>
+        <v>0.06896011256598221</v>
       </c>
       <c r="J16" s="12">
-        <v>0.05969448201893227</v>
+        <v>0.06833737515089292</v>
       </c>
       <c r="K16" s="12">
-        <v>0.05969448201893227</v>
+        <v>0.06771463773580363</v>
       </c>
       <c r="L16" s="12">
-        <v>0.05969448201893227</v>
+        <v>0.06709190032071434</v>
       </c>
       <c r="M16" s="13">
-        <v>0.05969448201893227</v>
+        <v>0.06646916290562505</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="10">
-        <v>0.05969448201893227</v>
+        <v>0.06584642549053575</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -3070,34 +3074,34 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="11">
-        <v>0.9436682147243023</v>
+        <v>0.9349439363371402</v>
       </c>
       <c r="E17" s="12">
-        <v>0.8905096994809518</v>
+        <v>0.8741201640935865</v>
       </c>
       <c r="F17" s="12">
-        <v>0.8403456983038647</v>
+        <v>0.8172533470493247</v>
       </c>
       <c r="G17" s="12">
-        <v>0.7930075248696552</v>
+        <v>0.7640860612749987</v>
       </c>
       <c r="H17" s="12">
-        <v>0.7483359952566853</v>
+        <v>0.7143776298287886</v>
       </c>
       <c r="I17" s="12">
-        <v>0.7061808926578101</v>
+        <v>0.6682921293610881</v>
       </c>
       <c r="J17" s="12">
-        <v>0.6664004622468098</v>
+        <v>0.6255440883238761</v>
       </c>
       <c r="K17" s="12">
-        <v>0.6288609344998968</v>
+        <v>0.5858719794742211</v>
       </c>
       <c r="L17" s="12">
-        <v>0.5934360753693739</v>
+        <v>0.5490361039177013</v>
       </c>
       <c r="M17" s="13">
-        <v>0.5600067617968135</v>
+        <v>0.5148166707622722</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="10" t="s">
@@ -3113,38 +3117,38 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="16">
-        <v>25638640.36095433</v>
+        <v>389203597.4127252</v>
       </c>
       <c r="E18" s="17">
-        <v>32797505.76917061</v>
+        <v>-3468294782.288646</v>
       </c>
       <c r="F18" s="17">
-        <v>40248060.00800606</v>
+        <v>-9154709225.152796</v>
       </c>
       <c r="G18" s="17">
-        <v>46237277.71961281</v>
+        <v>-17315289436.28718</v>
       </c>
       <c r="H18" s="17">
-        <v>47044246.91925912</v>
+        <v>-28797244020.94667</v>
       </c>
       <c r="I18" s="17">
-        <v>179131795.9412148</v>
+        <v>-12144066130.39416</v>
       </c>
       <c r="J18" s="17">
-        <v>412052617.4439876</v>
+        <v>13401842368.73143</v>
       </c>
       <c r="K18" s="17">
-        <v>761109381.0597914</v>
+        <v>47085051085.50179</v>
       </c>
       <c r="L18" s="17">
-        <v>1208709243.379211</v>
+        <v>86372925809.3085</v>
       </c>
       <c r="M18" s="18">
-        <v>1690586224.23282</v>
+        <v>127050199535.3275</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="15">
-        <v>52253513832.57134</v>
+        <v>3582582935638.691</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -3157,7 +3161,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="19">
-        <v>4443554992.834028</v>
+        <v>203419618801.2125</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -3165,7 +3169,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="19">
-        <v>52253513832.57134</v>
+        <v>3582582935638.691</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -3173,7 +3177,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="15">
-        <v>56697068825.40537</v>
+        <v>3786002554439.904</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -3181,7 +3185,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="19">
-        <v>151728000</v>
+        <v>28109000704</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -3197,7 +3201,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="19">
-        <v>90864000</v>
+        <v>142002995200</v>
       </c>
     </row>
     <row r="27" spans="1:15">
@@ -3213,7 +3217,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="15">
-        <v>56636204825.40537</v>
+        <v>3899896548935.904</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -3221,7 +3225,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="19">
-        <v>2460705024</v>
+        <v>1853588504576</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -3229,7 +3233,7 @@
         <v>28</v>
       </c>
       <c r="B30" s="19">
-        <v>126190000</v>
+        <v>317737984</v>
       </c>
     </row>
     <row r="31" spans="1:15">
@@ -3237,7 +3241,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="25">
-        <v>448.8169016990678</v>
+        <v>12273.93873354438</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -3245,7 +3249,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="27">
-        <v>19.5</v>
+        <v>2795.73</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -3253,7 +3257,818 @@
         <v>31</v>
       </c>
       <c r="B33" s="29">
-        <v>23.01625136918297</v>
+        <v>4.390244670817417</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr>
+    <tabColor rgb="FF93E100"/>
+  </sheetPr>
+  <dimension ref="A1:O33"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="4" max="13" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="25" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+    </row>
+    <row r="2" spans="1:15" ht="22" customHeight="1"/>
+    <row r="3" spans="1:15">
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="A4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5">
+        <v>44469</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7">
+        <v>44834</v>
+      </c>
+      <c r="E4" s="4">
+        <v>45199</v>
+      </c>
+      <c r="F4" s="4">
+        <v>45565</v>
+      </c>
+      <c r="G4" s="4">
+        <v>45930</v>
+      </c>
+      <c r="H4" s="4">
+        <v>46295</v>
+      </c>
+      <c r="I4" s="4">
+        <v>46660</v>
+      </c>
+      <c r="J4" s="4">
+        <v>47026</v>
+      </c>
+      <c r="K4" s="4">
+        <v>47391</v>
+      </c>
+      <c r="L4" s="4">
+        <v>47756</v>
+      </c>
+      <c r="M4" s="8">
+        <v>48121</v>
+      </c>
+      <c r="N4" s="6"/>
+      <c r="O4" s="5">
+        <v>48487</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0.32</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="11">
+        <v>0.26465</v>
+      </c>
+      <c r="E5" s="12">
+        <v>0.26465</v>
+      </c>
+      <c r="F5" s="12">
+        <v>0.26465</v>
+      </c>
+      <c r="G5" s="12">
+        <v>0.26465</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0.26465</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0.2233933335</v>
+      </c>
+      <c r="J5" s="12">
+        <v>0.182136667</v>
+      </c>
+      <c r="K5" s="12">
+        <v>0.1408800005</v>
+      </c>
+      <c r="L5" s="12">
+        <v>0.09962333399999998</v>
+      </c>
+      <c r="M5" s="13">
+        <v>0.05836666749999997</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="10">
+        <v>0.017110001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="15">
+        <v>511997000</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="16">
+        <v>647497006.0500001</v>
+      </c>
+      <c r="E6" s="17">
+        <v>818857088.7011327</v>
+      </c>
+      <c r="F6" s="17">
+        <v>1035567617.225887</v>
+      </c>
+      <c r="G6" s="17">
+        <v>1309630587.124719</v>
+      </c>
+      <c r="H6" s="17">
+        <v>1656224322.007276</v>
+      </c>
+      <c r="I6" s="17">
+        <v>2026213794.324258</v>
+      </c>
+      <c r="J6" s="17">
+        <v>2395261621.451902</v>
+      </c>
+      <c r="K6" s="17">
+        <v>2732706079.879677</v>
+      </c>
+      <c r="L6" s="17">
+        <v>3004947370.39936</v>
+      </c>
+      <c r="M6" s="18">
+        <v>3180336134.422459</v>
+      </c>
+      <c r="N6" s="6"/>
+      <c r="O6" s="15">
+        <v>3234751688.862764</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="10">
+        <v>-0.2097688072391049</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="11">
+        <v>-0.1552615489478042</v>
+      </c>
+      <c r="E7" s="12">
+        <v>-0.1007542906565035</v>
+      </c>
+      <c r="F7" s="12">
+        <v>-0.04624703236520281</v>
+      </c>
+      <c r="G7" s="12">
+        <v>0.008260225926097903</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0.06276748421739858</v>
+      </c>
+      <c r="I7" s="12">
+        <v>0.1172747425086993</v>
+      </c>
+      <c r="J7" s="12">
+        <v>0.1717820008</v>
+      </c>
+      <c r="K7" s="12">
+        <v>0.1717820008</v>
+      </c>
+      <c r="L7" s="12">
+        <v>0.1717820008</v>
+      </c>
+      <c r="M7" s="13">
+        <v>0.1717820008</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="10">
+        <v>0.1717820008</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="15">
+        <v>-107401000</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="16">
+        <v>-100531388.0983888</v>
+      </c>
+      <c r="E8" s="17">
+        <v>-82503365.12113219</v>
+      </c>
+      <c r="F8" s="17">
+        <v>-47891929.11020157</v>
+      </c>
+      <c r="G8" s="17">
+        <v>10817844.52937842</v>
+      </c>
+      <c r="H8" s="17">
+        <v>103957033.9920633</v>
+      </c>
+      <c r="I8" s="17">
+        <v>237623700.996952</v>
+      </c>
+      <c r="J8" s="17">
+        <v>411462833.77246</v>
+      </c>
+      <c r="K8" s="17">
+        <v>469429718.0000555</v>
+      </c>
+      <c r="L8" s="17">
+        <v>516195871.5859008</v>
+      </c>
+      <c r="M8" s="18">
+        <v>546324504.3876278</v>
+      </c>
+      <c r="N8" s="6"/>
+      <c r="O8" s="15">
+        <v>555672117.2040247</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="19">
+        <v>0</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="20">
+        <v>107401000</v>
+      </c>
+      <c r="E9" s="21">
+        <v>207932388.0983888</v>
+      </c>
+      <c r="F9" s="21">
+        <v>290435753.2195209</v>
+      </c>
+      <c r="G9" s="21">
+        <v>338327682.3297225</v>
+      </c>
+      <c r="H9" s="21">
+        <v>327509837.8003441</v>
+      </c>
+      <c r="I9" s="21">
+        <v>223552803.8082808</v>
+      </c>
+      <c r="J9" s="21">
+        <v>0</v>
+      </c>
+      <c r="K9" s="21">
+        <v>0</v>
+      </c>
+      <c r="L9" s="21">
+        <v>0</v>
+      </c>
+      <c r="M9" s="22">
+        <v>0</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="O9" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="19">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="20">
+        <v>0</v>
+      </c>
+      <c r="E10" s="21">
+        <v>0</v>
+      </c>
+      <c r="F10" s="21">
+        <v>0</v>
+      </c>
+      <c r="G10" s="21">
+        <v>0</v>
+      </c>
+      <c r="H10" s="21">
+        <v>0</v>
+      </c>
+      <c r="I10" s="21">
+        <v>14070897.18867123</v>
+      </c>
+      <c r="J10" s="21">
+        <v>411462833.77246</v>
+      </c>
+      <c r="K10" s="21">
+        <v>469429718.0000555</v>
+      </c>
+      <c r="L10" s="21">
+        <v>516195871.5859008</v>
+      </c>
+      <c r="M10" s="22">
+        <v>546324504.3876278</v>
+      </c>
+      <c r="N10" s="6"/>
+      <c r="O10" s="19">
+        <v>555672117.2040247</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="10">
+        <v>0.24</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="11">
+        <v>0.24</v>
+      </c>
+      <c r="E11" s="12">
+        <v>0.24</v>
+      </c>
+      <c r="F11" s="12">
+        <v>0.24</v>
+      </c>
+      <c r="G11" s="12">
+        <v>0.24</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0.24</v>
+      </c>
+      <c r="I11" s="12">
+        <v>0.24</v>
+      </c>
+      <c r="J11" s="12">
+        <v>0.24</v>
+      </c>
+      <c r="K11" s="12">
+        <v>0.24</v>
+      </c>
+      <c r="L11" s="12">
+        <v>0.24</v>
+      </c>
+      <c r="M11" s="13">
+        <v>0.24</v>
+      </c>
+      <c r="N11" s="6"/>
+      <c r="O11" s="10">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="15">
+        <v>-107401000</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="16">
+        <v>-100531388.0983888</v>
+      </c>
+      <c r="E12" s="17">
+        <v>-82503365.12113219</v>
+      </c>
+      <c r="F12" s="17">
+        <v>-47891929.11020157</v>
+      </c>
+      <c r="G12" s="17">
+        <v>10817844.52937842</v>
+      </c>
+      <c r="H12" s="17">
+        <v>103957033.9920633</v>
+      </c>
+      <c r="I12" s="17">
+        <v>234246685.6716709</v>
+      </c>
+      <c r="J12" s="17">
+        <v>312711753.6670696</v>
+      </c>
+      <c r="K12" s="17">
+        <v>356766585.6800421</v>
+      </c>
+      <c r="L12" s="17">
+        <v>392308862.4052846</v>
+      </c>
+      <c r="M12" s="18">
+        <v>415206623.3345972</v>
+      </c>
+      <c r="N12" s="6"/>
+      <c r="O12" s="15">
+        <v>422310809.0750588</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="10">
+        <v>4.575272890076471</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="11">
+        <v>4.575272890076471</v>
+      </c>
+      <c r="E13" s="12">
+        <v>4.575272890076471</v>
+      </c>
+      <c r="F13" s="12">
+        <v>4.575272890076471</v>
+      </c>
+      <c r="G13" s="12">
+        <v>4.575272890076471</v>
+      </c>
+      <c r="H13" s="12">
+        <v>4.575272890076471</v>
+      </c>
+      <c r="I13" s="12">
+        <v>4.575272890076471</v>
+      </c>
+      <c r="J13" s="12">
+        <v>4.575272890076471</v>
+      </c>
+      <c r="K13" s="12">
+        <v>4.575272890076471</v>
+      </c>
+      <c r="L13" s="12">
+        <v>4.575272890076471</v>
+      </c>
+      <c r="M13" s="13">
+        <v>4.575272890076471</v>
+      </c>
+      <c r="N13" s="6"/>
+      <c r="O13" s="10">
+        <v>4.575272890076471</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="19">
+        <v>0</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="20">
+        <v>29615721.13958329</v>
+      </c>
+      <c r="E14" s="21">
+        <v>37453521.739174</v>
+      </c>
+      <c r="F14" s="21">
+        <v>47365596.26744639</v>
+      </c>
+      <c r="G14" s="21">
+        <v>59900901.31962611</v>
+      </c>
+      <c r="H14" s="21">
+        <v>75753674.85386515</v>
+      </c>
+      <c r="I14" s="21">
+        <v>80867192.23228644</v>
+      </c>
+      <c r="J14" s="21">
+        <v>80661380.42346929</v>
+      </c>
+      <c r="K14" s="21">
+        <v>73753952.28548528</v>
+      </c>
+      <c r="L14" s="21">
+        <v>59502743.78390862</v>
+      </c>
+      <c r="M14" s="22">
+        <v>38334055.309249</v>
+      </c>
+      <c r="N14" s="6"/>
+      <c r="O14" s="19">
+        <v>11893400.84136386</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="16">
+        <v>-130147109.2379721</v>
+      </c>
+      <c r="E15" s="17">
+        <v>-119956886.8603062</v>
+      </c>
+      <c r="F15" s="17">
+        <v>-95257525.37764797</v>
+      </c>
+      <c r="G15" s="17">
+        <v>-49083056.79024769</v>
+      </c>
+      <c r="H15" s="17">
+        <v>28203359.1381982</v>
+      </c>
+      <c r="I15" s="17">
+        <v>153379493.4393845</v>
+      </c>
+      <c r="J15" s="17">
+        <v>232050373.2436002</v>
+      </c>
+      <c r="K15" s="17">
+        <v>283012633.3945569</v>
+      </c>
+      <c r="L15" s="17">
+        <v>332806118.621376</v>
+      </c>
+      <c r="M15" s="18">
+        <v>376872568.0253482</v>
+      </c>
+      <c r="N15" s="6"/>
+      <c r="O15" s="15">
+        <v>410417408.2336949</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="10">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="11">
+        <v>0.06530571184897939</v>
+      </c>
+      <c r="E16" s="12">
+        <v>0.06530571184897939</v>
+      </c>
+      <c r="F16" s="12">
+        <v>0.06530571184897939</v>
+      </c>
+      <c r="G16" s="12">
+        <v>0.06530571184897939</v>
+      </c>
+      <c r="H16" s="12">
+        <v>0.06530571184897939</v>
+      </c>
+      <c r="I16" s="12">
+        <v>0.06503940261156443</v>
+      </c>
+      <c r="J16" s="12">
+        <v>0.06477309337414949</v>
+      </c>
+      <c r="K16" s="12">
+        <v>0.06450678413673455</v>
+      </c>
+      <c r="L16" s="12">
+        <v>0.0642404748993196</v>
+      </c>
+      <c r="M16" s="13">
+        <v>0.06397416566190464</v>
+      </c>
+      <c r="N16" s="6"/>
+      <c r="O16" s="10">
+        <v>0.0637078564244897</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="10">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="11">
+        <v>0.9386976798090825</v>
+      </c>
+      <c r="E17" s="12">
+        <v>0.8811533340789547</v>
+      </c>
+      <c r="F17" s="12">
+        <v>0.8271365902559521</v>
+      </c>
+      <c r="G17" s="12">
+        <v>0.776431198158458</v>
+      </c>
+      <c r="H17" s="12">
+        <v>0.7288341642427304</v>
+      </c>
+      <c r="I17" s="12">
+        <v>0.6843260093998109</v>
+      </c>
+      <c r="J17" s="12">
+        <v>0.6426965647969716</v>
+      </c>
+      <c r="K17" s="12">
+        <v>0.6037505578869266</v>
+      </c>
+      <c r="L17" s="12">
+        <v>0.5673065177717876</v>
+      </c>
+      <c r="M17" s="13">
+        <v>0.5331957636573468</v>
+      </c>
+      <c r="N17" s="6"/>
+      <c r="O17" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="16">
+        <v>-122168789.4755436</v>
+      </c>
+      <c r="E18" s="17">
+        <v>-105700410.8026908</v>
+      </c>
+      <c r="F18" s="17">
+        <v>-78790984.73708756</v>
+      </c>
+      <c r="G18" s="17">
+        <v>-38109616.59293164</v>
+      </c>
+      <c r="H18" s="17">
+        <v>20555571.68632625</v>
+      </c>
+      <c r="I18" s="17">
+        <v>104961576.6691384</v>
+      </c>
+      <c r="J18" s="17">
+        <v>149137977.743517</v>
+      </c>
+      <c r="K18" s="17">
+        <v>170869035.3010119</v>
+      </c>
+      <c r="L18" s="17">
+        <v>188803080.2482373</v>
+      </c>
+      <c r="M18" s="18">
+        <v>200946856.7097809</v>
+      </c>
+      <c r="N18" s="6"/>
+      <c r="O18" s="15">
+        <v>4696199458.278621</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="B20" s="23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="19">
+        <v>490504296.7497582</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="19">
+        <v>4696199458.278621</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="15">
+        <v>5186703755.028379</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="19">
+        <v>266236992</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
+      <c r="A28" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="15">
+        <v>5452940747.028379</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
+      <c r="A29" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="19">
+        <v>3878781440</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="A30" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="19">
+        <v>94129696</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
+      <c r="A31" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31" s="25">
+        <v>57.9300792284337</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
+      <c r="A32" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="27">
+        <v>34.27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="29">
+        <v>1.690402078448605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran pylint through all scripts and cleaned up code, renamed files to final names, separated excel formatter to separate script, changed Excel output color format, updated README tables and images
</commit_message>
<xml_diff>
--- a/DCF valuations.xlsx
+++ b/DCF valuations.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="36">
   <si>
-    <t>Valuation of Asana, Inc. on 2022-01-16</t>
+    <t>Valuation of Asana, Inc. on 2022-01-17</t>
   </si>
   <si>
     <t>Year Ended</t>
@@ -118,13 +118,13 @@
     <t>--</t>
   </si>
   <si>
-    <t>Valuation of Salesforce.com Inc on 2022-01-16</t>
+    <t>Valuation of Salesforce.com Inc on 2022-01-17</t>
   </si>
   <si>
-    <t>Valuation of Alphabet Inc. on 2022-01-16</t>
+    <t>Valuation of Alphabet Inc. on 2022-01-17</t>
   </si>
   <si>
-    <t>Valuation of Warby Parker Inc. on 2022-01-16</t>
+    <t>Valuation of Warby Parker Inc. on 2022-01-17</t>
   </si>
 </sst>
 </file>
@@ -173,7 +173,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -181,7 +181,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -196,25 +196,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF58F00"/>
+        <fgColor rgb="FF2675CC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF2066A6"/>
+        <fgColor rgb="FF333F4F"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC9C9CB"/>
+        <fgColor rgb="FFEDEDED"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFE9CA"/>
+        <fgColor rgb="FFD3E3F5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -226,18 +226,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF77777D"/>
+        <fgColor rgb="FF222B35"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF3188D7"/>
+        <fgColor rgb="FF1F4D82"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -434,6 +434,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -467,24 +476,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -500,17 +509,17 @@
     <xf numFmtId="165" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="2" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="6" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="3" fillId="6" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -525,19 +534,20 @@
     <xf numFmtId="166" fontId="0" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="3" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="3" fillId="8" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="2" fillId="8" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="3" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -835,7 +845,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <tabColor rgb="FFE19800"/>
+    <tabColor rgb="FFE18D00"/>
   </sheetPr>
   <dimension ref="A1:O33"/>
   <sheetViews>
@@ -850,9 +860,9 @@
   <cols>
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
     <col min="4" max="13" width="14.7109375" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1"/>
+    <col min="14" max="14" width="5.7109375" customWidth="1"/>
     <col min="15" max="15" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -951,23 +961,23 @@
         <v>0.5610999999999999</v>
       </c>
       <c r="I5" s="12">
-        <v>0.4704350001666666</v>
+        <v>0.4704349999999999</v>
       </c>
       <c r="J5" s="12">
-        <v>0.3797700003333333</v>
+        <v>0.3797699999999999</v>
       </c>
       <c r="K5" s="12">
-        <v>0.2891050005</v>
+        <v>0.2891049999999999</v>
       </c>
       <c r="L5" s="12">
-        <v>0.1984400006666667</v>
+        <v>0.1984399999999999</v>
       </c>
       <c r="M5" s="13">
-        <v>0.1077750008333334</v>
+        <v>0.107775</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="10">
-        <v>0.017110001</v>
+        <v>0.01711</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -994,23 +1004,23 @@
         <v>3104652525.092923</v>
       </c>
       <c r="I6" s="17">
-        <v>4565189736.252454</v>
+        <v>4565189735.735011</v>
       </c>
       <c r="J6" s="17">
-        <v>6298911843.910778</v>
+        <v>6298911841.675096</v>
       </c>
       <c r="K6" s="17">
-        <v>8119958755.694059</v>
+        <v>8119958749.662574</v>
       </c>
       <c r="L6" s="17">
-        <v>9731283376.587294</v>
+        <v>9731283363.945614</v>
       </c>
       <c r="M6" s="18">
-        <v>10780072450.60839</v>
+        <v>10780072428.49485</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="15">
-        <v>10964519501.01838</v>
+        <v>10964519467.7464</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1080,23 +1090,23 @@
         <v>-722451400.3353819</v>
       </c>
       <c r="I8" s="17">
-        <v>-650146700.6941097</v>
+        <v>-650146700.6204185</v>
       </c>
       <c r="J8" s="17">
-        <v>-328351561.1503511</v>
+        <v>-328351561.0338088</v>
       </c>
       <c r="K8" s="17">
-        <v>309836117.6183255</v>
+        <v>309836117.38818</v>
       </c>
       <c r="L8" s="17">
-        <v>1249915245.335927</v>
+        <v>1249915243.712191</v>
       </c>
       <c r="M8" s="18">
-        <v>1384624861.943602</v>
+        <v>1384624859.103273</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="15">
-        <v>1408315794.716082</v>
+        <v>1408315790.44253</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1126,20 +1136,20 @@
         <v>2841721219.956268</v>
       </c>
       <c r="J9" s="21">
-        <v>3491867920.650377</v>
+        <v>3491867920.576686</v>
       </c>
       <c r="K9" s="21">
-        <v>3820219481.800728</v>
+        <v>3820219481.610495</v>
       </c>
       <c r="L9" s="21">
-        <v>3510383364.182403</v>
+        <v>3510383364.222315</v>
       </c>
       <c r="M9" s="22">
-        <v>2260468118.846476</v>
+        <v>2260468120.510124</v>
       </c>
       <c r="N9" s="6"/>
       <c r="O9" s="19">
-        <v>875843256.9028733</v>
+        <v>875843261.4068515</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1182,7 +1192,7 @@
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="19">
-        <v>532472537.8132091</v>
+        <v>532472529.0356781</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1252,23 +1262,23 @@
         <v>-722451400.3353819</v>
       </c>
       <c r="I12" s="17">
-        <v>-650146700.6941097</v>
+        <v>-650146700.6204185</v>
       </c>
       <c r="J12" s="17">
-        <v>-328351561.1503511</v>
+        <v>-328351561.0338088</v>
       </c>
       <c r="K12" s="17">
-        <v>309836117.6183255</v>
+        <v>309836117.38818</v>
       </c>
       <c r="L12" s="17">
-        <v>1249915245.335927</v>
+        <v>1249915243.712191</v>
       </c>
       <c r="M12" s="18">
-        <v>1384624861.943602</v>
+        <v>1384624859.103273</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="15">
-        <v>1280522385.640912</v>
+        <v>1280522383.473967</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1338,23 +1348,23 @@
         <v>884270596.9261782</v>
       </c>
       <c r="I14" s="21">
-        <v>1157378112.538785</v>
+        <v>1157378112.128746</v>
       </c>
       <c r="J14" s="21">
-        <v>1373858882.400759</v>
+        <v>1373858881.039169</v>
       </c>
       <c r="K14" s="21">
-        <v>1443057952.581055</v>
+        <v>1443057949.573134</v>
       </c>
       <c r="L14" s="21">
-        <v>1276867055.606284</v>
+        <v>1276867050.368147</v>
       </c>
       <c r="M14" s="22">
-        <v>831095236.5110632</v>
+        <v>831095229.0052466</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="19">
-        <v>146161958.3778851</v>
+        <v>146161949.5355706</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1381,23 +1391,23 @@
         <v>-1606721997.26156</v>
       </c>
       <c r="I15" s="17">
-        <v>-1807524813.232894</v>
+        <v>-1807524812.749164</v>
       </c>
       <c r="J15" s="17">
-        <v>-1702210443.55111</v>
+        <v>-1702210442.072978</v>
       </c>
       <c r="K15" s="17">
-        <v>-1133221834.962729</v>
+        <v>-1133221832.184954</v>
       </c>
       <c r="L15" s="17">
-        <v>-26951810.27035713</v>
+        <v>-26951806.65595555</v>
       </c>
       <c r="M15" s="18">
-        <v>553529625.4325391</v>
+        <v>553529630.098026</v>
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="15">
-        <v>1134360427.263027</v>
+        <v>1134360433.938396</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1409,38 +1419,38 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="11">
-        <v>0.07514240345993498</v>
+        <v>0.07628218674670335</v>
       </c>
       <c r="E16" s="12">
-        <v>0.07514240345993498</v>
+        <v>0.07628218674670335</v>
       </c>
       <c r="F16" s="12">
-        <v>0.07514240345993498</v>
+        <v>0.07628218674670335</v>
       </c>
       <c r="G16" s="12">
-        <v>0.07514240345993498</v>
+        <v>0.07628218674670335</v>
       </c>
       <c r="H16" s="12">
-        <v>0.07514240345993498</v>
+        <v>0.07628218674670335</v>
       </c>
       <c r="I16" s="12">
-        <v>0.07405636992160707</v>
+        <v>0.07510117118447807</v>
       </c>
       <c r="J16" s="12">
-        <v>0.07297033638327914</v>
+        <v>0.07392015562225279</v>
       </c>
       <c r="K16" s="12">
-        <v>0.07188430284495123</v>
+        <v>0.07273914006002752</v>
       </c>
       <c r="L16" s="12">
-        <v>0.07079826930662332</v>
+        <v>0.07155812449780223</v>
       </c>
       <c r="M16" s="13">
-        <v>0.0697122357682954</v>
+        <v>0.07037710893557694</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="10">
-        <v>0.06862620222996749</v>
+        <v>0.06919609337335167</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1452,34 +1462,34 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="11">
-        <v>0.9301093481029881</v>
+        <v>0.9291243619135955</v>
       </c>
       <c r="E17" s="12">
-        <v>0.8651033994285654</v>
+        <v>0.8632720799013459</v>
       </c>
       <c r="F17" s="12">
-        <v>0.8046407588841819</v>
+        <v>0.8020871203961605</v>
       </c>
       <c r="G17" s="12">
-        <v>0.74840389170286</v>
+        <v>0.7452386839371958</v>
       </c>
       <c r="H17" s="12">
-        <v>0.6960974558294865</v>
+        <v>0.6924194166864748</v>
       </c>
       <c r="I17" s="12">
-        <v>0.6481014175078101</v>
+        <v>0.6440504719417347</v>
       </c>
       <c r="J17" s="12">
-        <v>0.6040254753849036</v>
+        <v>0.5997191397982076</v>
       </c>
       <c r="K17" s="12">
-        <v>0.5635174186073292</v>
+        <v>0.5590540303811875</v>
       </c>
       <c r="L17" s="12">
-        <v>0.5262591794925341</v>
+        <v>0.521720677208429</v>
       </c>
       <c r="M17" s="13">
-        <v>0.491963316764869</v>
+        <v>0.4874176333304134</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="10" t="s">
@@ -1495,42 +1505,43 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="16">
-        <v>-427215115.9794217</v>
+        <v>-426762694.9925799</v>
       </c>
       <c r="E18" s="17">
-        <v>-556574315.9309331</v>
+        <v>-555396115.2513537</v>
       </c>
       <c r="F18" s="17">
-        <v>-715593278.2925193</v>
+        <v>-713322244.2726279</v>
       </c>
       <c r="G18" s="17">
-        <v>-904656189.1128662</v>
+        <v>-900830147.0161034</v>
       </c>
       <c r="H18" s="17">
-        <v>-1118435094.519043</v>
+        <v>-1112525508.121177</v>
       </c>
       <c r="I18" s="17">
-        <v>-1171459393.636779</v>
+        <v>-1164137208.697495</v>
       </c>
       <c r="J18" s="17">
-        <v>-1028178472.371107</v>
+        <v>-1020848182.075533</v>
       </c>
       <c r="K18" s="17">
-        <v>-638590243.147658</v>
+        <v>-633532232.5989524</v>
       </c>
       <c r="L18" s="17">
-        <v>-14183637.5587166</v>
+        <v>-14061314.82053577</v>
       </c>
       <c r="M18" s="18">
-        <v>272316270.4554075</v>
+        <v>269800102.280639</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="15">
-        <v>10832780851.05587</v>
+        <v>10615257206.76899</v>
       </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="23"/>
+      <c r="B20" s="24" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1539,7 +1550,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="19">
-        <v>-6302569470.093637</v>
+        <v>-6271615545.565719</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1547,7 +1558,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="19">
-        <v>10832780851.05587</v>
+        <v>10615257206.76899</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1555,7 +1566,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="15">
-        <v>4530211380.962234</v>
+        <v>4343641661.203271</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1595,7 +1606,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="15">
-        <v>4618517380.962234</v>
+        <v>4431947661.203271</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -1615,27 +1626,27 @@
       </c>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="25">
-        <v>47.27708537340654</v>
+      <c r="B31" s="26">
+        <v>45.36727929462128</v>
       </c>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="27">
+      <c r="B32" s="28">
         <v>60.18</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="29">
-        <v>0.7855946389731894</v>
+      <c r="B33" s="30">
+        <v>0.7538597423499714</v>
       </c>
     </row>
   </sheetData>
@@ -1661,9 +1672,9 @@
   <cols>
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
     <col min="4" max="13" width="14.7109375" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1"/>
+    <col min="14" max="14" width="5.7109375" customWidth="1"/>
     <col min="15" max="15" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1762,23 +1773,23 @@
         <v>0.2546410854503579</v>
       </c>
       <c r="I5" s="12">
-        <v>0.2150525713752983</v>
+        <v>0.2150525712086316</v>
       </c>
       <c r="J5" s="12">
-        <v>0.1754640573002386</v>
+        <v>0.1754640569669053</v>
       </c>
       <c r="K5" s="12">
-        <v>0.1358755432251789</v>
+        <v>0.135875542725179</v>
       </c>
       <c r="L5" s="12">
-        <v>0.0962870291501193</v>
+        <v>0.09628702848345264</v>
       </c>
       <c r="M5" s="13">
-        <v>0.05669851507505966</v>
+        <v>0.05669851424172631</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="10">
-        <v>0.017110001</v>
+        <v>0.01711</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1805,23 +1816,23 @@
         <v>77667998554.88492</v>
       </c>
       <c r="I6" s="17">
-        <v>94370701357.68587</v>
+        <v>94370701344.7412</v>
       </c>
       <c r="J6" s="17">
-        <v>110929367508.1746</v>
+        <v>110929367461.5017</v>
       </c>
       <c r="K6" s="17">
-        <v>126001955577.9733</v>
+        <v>126001955469.494</v>
       </c>
       <c r="L6" s="17">
-        <v>138134309547.6816</v>
+        <v>138134309344.7559</v>
       </c>
       <c r="M6" s="18">
-        <v>145966319779.9538</v>
+        <v>145966319450.4106</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="15">
-        <v>148463803657.3552</v>
+        <v>148463803176.2071</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1891,23 +1902,23 @@
         <v>8816372006.531195</v>
       </c>
       <c r="I8" s="17">
-        <v>12121256136.0413</v>
+        <v>12121256134.37864</v>
       </c>
       <c r="J8" s="17">
-        <v>14248100917.24652</v>
+        <v>14248100911.25171</v>
       </c>
       <c r="K8" s="17">
-        <v>16184069369.30456</v>
+        <v>16184069355.37115</v>
       </c>
       <c r="L8" s="17">
-        <v>17742385328.43433</v>
+        <v>17742385302.36995</v>
       </c>
       <c r="M8" s="18">
-        <v>18748352230.44609</v>
+        <v>18748352188.11856</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="15">
-        <v>19069136555.85737</v>
+        <v>19069136494.05727</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1977,23 +1988,23 @@
         <v>8816372006.531195</v>
       </c>
       <c r="I10" s="21">
-        <v>12121256136.0413</v>
+        <v>12121256134.37864</v>
       </c>
       <c r="J10" s="21">
-        <v>14248100917.24652</v>
+        <v>14248100911.25171</v>
       </c>
       <c r="K10" s="21">
-        <v>16184069369.30456</v>
+        <v>16184069355.37115</v>
       </c>
       <c r="L10" s="21">
-        <v>17742385328.43433</v>
+        <v>17742385302.36995</v>
       </c>
       <c r="M10" s="22">
-        <v>18748352230.44609</v>
+        <v>18748352188.11856</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="19">
-        <v>19069136555.85737</v>
+        <v>19069136494.05727</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -2063,23 +2074,23 @@
         <v>6700442724.963708</v>
       </c>
       <c r="I12" s="17">
-        <v>9212154663.391384</v>
+        <v>9212154662.127769</v>
       </c>
       <c r="J12" s="17">
-        <v>10828556697.10735</v>
+        <v>10828556692.5513</v>
       </c>
       <c r="K12" s="17">
-        <v>12299892720.67146</v>
+        <v>12299892710.08208</v>
       </c>
       <c r="L12" s="17">
-        <v>13484212849.61009</v>
+        <v>13484212829.80116</v>
       </c>
       <c r="M12" s="18">
-        <v>14248747695.13903</v>
+        <v>14248747662.97011</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="15">
-        <v>14492543782.4516</v>
+        <v>14492543735.48352</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -2149,23 +2160,23 @@
         <v>18272548994.35591</v>
       </c>
       <c r="I14" s="21">
-        <v>19361312874.01737</v>
+        <v>19361312859.01226</v>
       </c>
       <c r="J14" s="21">
-        <v>19194349555.34562</v>
+        <v>19194349516.24879</v>
       </c>
       <c r="K14" s="21">
-        <v>17471728790.60133</v>
+        <v>17471728718.95708</v>
       </c>
       <c r="L14" s="21">
-        <v>14063490435.00066</v>
+        <v>14063490325.52095</v>
       </c>
       <c r="M14" s="22">
-        <v>9078650463.330906</v>
+        <v>9078650316.559362</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="19">
-        <v>2895014496.700051</v>
+        <v>2895014320.963912</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -2192,23 +2203,23 @@
         <v>-11572106269.3922</v>
       </c>
       <c r="I15" s="17">
-        <v>-10149158210.62599</v>
+        <v>-10149158196.88449</v>
       </c>
       <c r="J15" s="17">
-        <v>-8365792858.238268</v>
+        <v>-8365792823.697493</v>
       </c>
       <c r="K15" s="17">
-        <v>-5171836069.929871</v>
+        <v>-5171836008.875006</v>
       </c>
       <c r="L15" s="17">
-        <v>-579277585.3905697</v>
+        <v>-579277495.7197914</v>
       </c>
       <c r="M15" s="18">
-        <v>5170097231.808121</v>
+        <v>5170097346.410746</v>
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="15">
-        <v>11597529285.75155</v>
+        <v>11597529414.51961</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -2220,38 +2231,38 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="11">
-        <v>0.07486139272426998</v>
+        <v>0.07598471660702244</v>
       </c>
       <c r="E16" s="12">
-        <v>0.07486139272426998</v>
+        <v>0.07598471660702244</v>
       </c>
       <c r="F16" s="12">
-        <v>0.07486139272426998</v>
+        <v>0.07598471660702244</v>
       </c>
       <c r="G16" s="12">
-        <v>0.07486139272426998</v>
+        <v>0.07598471660702244</v>
       </c>
       <c r="H16" s="12">
-        <v>0.07486139272426998</v>
+        <v>0.07598471660702244</v>
       </c>
       <c r="I16" s="12">
-        <v>0.07379877674724748</v>
+        <v>0.07482849022310391</v>
       </c>
       <c r="J16" s="12">
-        <v>0.07273616077022498</v>
+        <v>0.07367226383918536</v>
       </c>
       <c r="K16" s="12">
-        <v>0.07167354479320248</v>
+        <v>0.07251603745526683</v>
       </c>
       <c r="L16" s="12">
-        <v>0.07061092881617999</v>
+        <v>0.0713598110713483</v>
       </c>
       <c r="M16" s="13">
-        <v>0.06954831283915748</v>
+        <v>0.07020358468742975</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="10">
-        <v>0.06848569686213499</v>
+        <v>0.06904735830351122</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -2263,34 +2274,34 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="11">
-        <v>0.9303525150023935</v>
+        <v>0.9293812305748819</v>
       </c>
       <c r="E17" s="12">
-        <v>0.8655558021712788</v>
+        <v>0.8637494717448817</v>
       </c>
       <c r="F17" s="12">
-        <v>0.8052720174249633</v>
+        <v>0.8027525469586623</v>
       </c>
       <c r="G17" s="12">
-        <v>0.7491868466723659</v>
+        <v>0.7460631499395621</v>
       </c>
       <c r="H17" s="12">
-        <v>0.6970078670083482</v>
+        <v>0.6933770883774029</v>
       </c>
       <c r="I17" s="12">
-        <v>0.6491047318192382</v>
+        <v>0.6451048652734144</v>
       </c>
       <c r="J17" s="12">
-        <v>0.6050926178839545</v>
+        <v>0.6008396481871289</v>
       </c>
       <c r="K17" s="12">
-        <v>0.5646240133703379</v>
+        <v>0.5602150711076794</v>
       </c>
       <c r="L17" s="12">
-        <v>0.5273848773379014</v>
+        <v>0.5229009575666931</v>
       </c>
       <c r="M17" s="13">
-        <v>0.4930912152420098</v>
+        <v>0.4885995198001647</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="10" t="s">
@@ -2306,42 +2317,43 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="16">
-        <v>-5668435022.571997</v>
+        <v>-5662517198.331181</v>
       </c>
       <c r="E18" s="17">
-        <v>-6230308284.961009</v>
+        <v>-6217306240.040591</v>
       </c>
       <c r="F18" s="17">
-        <v>-6821560943.616257</v>
+        <v>-6800218191.155452</v>
       </c>
       <c r="G18" s="17">
-        <v>-7436302274.888277</v>
+        <v>-7405296987.991713</v>
       </c>
       <c r="H18" s="17">
-        <v>-8065849107.622991</v>
+        <v>-8023833351.465054</v>
       </c>
       <c r="I18" s="17">
-        <v>-6587866618.499402</v>
+        <v>-6547271331.239741</v>
       </c>
       <c r="J18" s="17">
-        <v>-5062079501.266284</v>
+        <v>-5026500016.996809</v>
       </c>
       <c r="K18" s="17">
-        <v>-2920142838.297279</v>
+        <v>-2897340477.469168</v>
       </c>
       <c r="L18" s="17">
-        <v>-305502238.3158013</v>
+        <v>-302904757.2087149</v>
       </c>
       <c r="M18" s="18">
-        <v>2549329526.951617</v>
+        <v>2526107080.776396</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="15">
-        <v>111310216111.9494</v>
+        <v>109103494823.2914</v>
       </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="23"/>
+      <c r="B20" s="24" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2350,7 +2362,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="19">
-        <v>-46548717303.08768</v>
+        <v>-46357081471.12202</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -2358,7 +2370,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="19">
-        <v>111310216111.9494</v>
+        <v>109103494823.2914</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -2366,7 +2378,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="15">
-        <v>64761498808.86175</v>
+        <v>62746413352.16937</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -2406,7 +2418,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="15">
-        <v>59814498488.86176</v>
+        <v>57799413032.16937</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -2426,27 +2438,27 @@
       </c>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="25">
-        <v>60.7253791765094</v>
+      <c r="B31" s="26">
+        <v>58.67960713925824</v>
       </c>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="27">
+      <c r="B32" s="28">
         <v>231.23</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="29">
-        <v>0.2626189472668313</v>
+      <c r="B33" s="30">
+        <v>0.2537716003081704</v>
       </c>
     </row>
   </sheetData>
@@ -2472,9 +2484,9 @@
   <cols>
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
     <col min="4" max="13" width="14.7109375" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1"/>
+    <col min="14" max="14" width="5.7109375" customWidth="1"/>
     <col min="15" max="15" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2573,23 +2585,23 @@
         <v>0.3201761451922981</v>
       </c>
       <c r="I5" s="12">
-        <v>0.2696651211602484</v>
+        <v>0.2696651209935818</v>
       </c>
       <c r="J5" s="12">
-        <v>0.2191540971281987</v>
+        <v>0.2191540967948654</v>
       </c>
       <c r="K5" s="12">
-        <v>0.168643073096149</v>
+        <v>0.1686430725961491</v>
       </c>
       <c r="L5" s="12">
-        <v>0.1181320490640994</v>
+        <v>0.1181320483974327</v>
       </c>
       <c r="M5" s="13">
-        <v>0.0676210250320497</v>
+        <v>0.06762102419871635</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="10">
-        <v>0.017110001</v>
+        <v>0.01711</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -2616,23 +2628,23 @@
         <v>959265303239.4132</v>
       </c>
       <c r="I6" s="17">
-        <v>1217945697462.292</v>
+        <v>1217945697302.414</v>
       </c>
       <c r="J6" s="17">
-        <v>1484863487140.815</v>
+        <v>1484863486539.917</v>
       </c>
       <c r="K6" s="17">
-        <v>1735275428740.506</v>
+        <v>1735275427295.84</v>
       </c>
       <c r="L6" s="17">
-        <v>1940267070828.205</v>
+        <v>1940267068056.027</v>
       </c>
       <c r="M6" s="18">
-        <v>2071469918993.541</v>
+        <v>2071469914417.016</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="15">
-        <v>2106912771378.991</v>
+        <v>2106912764652.691</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -2702,23 +2714,23 @@
         <v>222274179164.1181</v>
       </c>
       <c r="I8" s="17">
-        <v>282213772619.2047</v>
+        <v>282213772582.159</v>
       </c>
       <c r="J8" s="17">
-        <v>344062077154.7093</v>
+        <v>344062077015.4736</v>
       </c>
       <c r="K8" s="17">
-        <v>402085763181.9238</v>
+        <v>402085762847.1759</v>
       </c>
       <c r="L8" s="17">
-        <v>449584978286.1066</v>
+        <v>449584977643.7571</v>
       </c>
       <c r="M8" s="18">
-        <v>479986375356.825</v>
+        <v>479986374296.385</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="15">
-        <v>488198942719.1667</v>
+        <v>488198941160.5961</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -2788,23 +2800,23 @@
         <v>222274179164.1181</v>
       </c>
       <c r="I10" s="21">
-        <v>282213772619.2047</v>
+        <v>282213772582.159</v>
       </c>
       <c r="J10" s="21">
-        <v>344062077154.7093</v>
+        <v>344062077015.4736</v>
       </c>
       <c r="K10" s="21">
-        <v>402085763181.9238</v>
+        <v>402085762847.1759</v>
       </c>
       <c r="L10" s="21">
-        <v>449584978286.1066</v>
+        <v>449584977643.7571</v>
       </c>
       <c r="M10" s="22">
-        <v>479986375356.825</v>
+        <v>479986374296.385</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="19">
-        <v>488198942719.1667</v>
+        <v>488198941160.5961</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -2874,23 +2886,23 @@
         <v>168928376164.7297</v>
       </c>
       <c r="I12" s="17">
-        <v>214482467190.5956</v>
+        <v>214482467162.4409</v>
       </c>
       <c r="J12" s="17">
-        <v>261487178637.579</v>
+        <v>261487178531.7599</v>
       </c>
       <c r="K12" s="17">
-        <v>305585180018.2621</v>
+        <v>305585179763.8537</v>
       </c>
       <c r="L12" s="17">
-        <v>341684583497.441</v>
+        <v>341684583009.2554</v>
       </c>
       <c r="M12" s="18">
-        <v>364789645271.187</v>
+        <v>364789644465.2526</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="15">
-        <v>371031196466.5667</v>
+        <v>371031195282.0531</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -2960,23 +2972,23 @@
         <v>209239330509.4904</v>
       </c>
       <c r="I14" s="21">
-        <v>232654260029.162</v>
+        <v>232654259885.3698</v>
       </c>
       <c r="J14" s="21">
-        <v>240062881583.4078</v>
+        <v>240062881186.7598</v>
       </c>
       <c r="K14" s="21">
-        <v>225217706004.9848</v>
+        <v>225217705246.1083</v>
       </c>
       <c r="L14" s="21">
-        <v>184367195455.041</v>
+        <v>184367194261.0918</v>
       </c>
       <c r="M14" s="22">
-        <v>118002377587.7058</v>
+        <v>118002375964.8963</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="19">
-        <v>31876905939.59308</v>
+        <v>31876904006.10997</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -3003,23 +3015,23 @@
         <v>-40310954344.76071</v>
       </c>
       <c r="I15" s="17">
-        <v>-18171792838.56647</v>
+        <v>-18171792722.92899</v>
       </c>
       <c r="J15" s="17">
-        <v>21424297054.1712</v>
+        <v>21424297345.00015</v>
       </c>
       <c r="K15" s="17">
-        <v>80367474013.27728</v>
+        <v>80367474517.74536</v>
       </c>
       <c r="L15" s="17">
-        <v>157317388042.4001</v>
+        <v>157317388748.1637</v>
       </c>
       <c r="M15" s="18">
-        <v>246787267683.4812</v>
+        <v>246787268500.3563</v>
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="15">
-        <v>339154290526.9736</v>
+        <v>339154291275.9431</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -3031,38 +3043,38 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="11">
-        <v>0.0695828499810715</v>
+        <v>0.0706354870011382</v>
       </c>
       <c r="E16" s="12">
-        <v>0.0695828499810715</v>
+        <v>0.0706354870011382</v>
       </c>
       <c r="F16" s="12">
-        <v>0.0695828499810715</v>
+        <v>0.0706354870011382</v>
       </c>
       <c r="G16" s="12">
-        <v>0.0695828499810715</v>
+        <v>0.0706354870011382</v>
       </c>
       <c r="H16" s="12">
-        <v>0.0695828499810715</v>
+        <v>0.0706354870011382</v>
       </c>
       <c r="I16" s="12">
-        <v>0.06896011256598221</v>
+        <v>0.06992502975104335</v>
       </c>
       <c r="J16" s="12">
-        <v>0.06833737515089292</v>
+        <v>0.06921457250094849</v>
       </c>
       <c r="K16" s="12">
-        <v>0.06771463773580363</v>
+        <v>0.06850411525085365</v>
       </c>
       <c r="L16" s="12">
-        <v>0.06709190032071434</v>
+        <v>0.0677936580007588</v>
       </c>
       <c r="M16" s="13">
-        <v>0.06646916290562505</v>
+        <v>0.06708320075066394</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="10">
-        <v>0.06584642549053575</v>
+        <v>0.0663727435005691</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -3074,34 +3086,34 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="11">
-        <v>0.9349439363371402</v>
+        <v>0.934024709755335</v>
       </c>
       <c r="E17" s="12">
-        <v>0.8741201640935865</v>
+        <v>0.8724021584335379</v>
       </c>
       <c r="F17" s="12">
-        <v>0.8172533470493247</v>
+        <v>0.814845172820813</v>
       </c>
       <c r="G17" s="12">
-        <v>0.7640860612749987</v>
+        <v>0.7610855260394958</v>
       </c>
       <c r="H17" s="12">
-        <v>0.7143776298287886</v>
+        <v>0.7108726875580265</v>
       </c>
       <c r="I17" s="12">
-        <v>0.6682921293610881</v>
+        <v>0.6644135502871977</v>
       </c>
       <c r="J17" s="12">
-        <v>0.6255440883238761</v>
+        <v>0.6214033809257761</v>
       </c>
       <c r="K17" s="12">
-        <v>0.5858719794742211</v>
+        <v>0.5815638630272272</v>
       </c>
       <c r="L17" s="12">
-        <v>0.5490361039177013</v>
+        <v>0.5446406790953369</v>
       </c>
       <c r="M17" s="13">
-        <v>0.5148166707622722</v>
+        <v>0.510401324575438</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="10" t="s">
@@ -3117,42 +3129,43 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="16">
-        <v>389203597.4127252</v>
+        <v>388820936.7219916</v>
       </c>
       <c r="E18" s="17">
-        <v>-3468294782.288646</v>
+        <v>-3461478156.484266</v>
       </c>
       <c r="F18" s="17">
-        <v>-9154709225.152796</v>
+        <v>-9127733337.069708</v>
       </c>
       <c r="G18" s="17">
-        <v>-17315289436.28718</v>
+        <v>-17247292990.99172</v>
       </c>
       <c r="H18" s="17">
-        <v>-28797244020.94667</v>
+        <v>-28655956453.08895</v>
       </c>
       <c r="I18" s="17">
-        <v>-12144066130.39416</v>
+        <v>-12073585318.12431</v>
       </c>
       <c r="J18" s="17">
-        <v>13401842368.73143</v>
+        <v>13313130804.14222</v>
       </c>
       <c r="K18" s="17">
-        <v>47085051085.50179</v>
+        <v>46738818942.28223</v>
       </c>
       <c r="L18" s="17">
-        <v>86372925809.3085</v>
+        <v>85681449441.30496</v>
       </c>
       <c r="M18" s="18">
-        <v>127050199535.3275</v>
+        <v>125960548730.9361</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="15">
-        <v>3582582935638.691</v>
+        <v>3513909035551.086</v>
       </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="23"/>
+      <c r="B20" s="24" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3161,7 +3174,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="19">
-        <v>203419618801.2125</v>
+        <v>201516722599.6286</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -3169,7 +3182,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="19">
-        <v>3582582935638.691</v>
+        <v>3513909035551.086</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -3177,7 +3190,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="15">
-        <v>3786002554439.904</v>
+        <v>3715425758150.714</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -3217,7 +3230,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="15">
-        <v>3899896548935.904</v>
+        <v>3829319752646.714</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -3237,27 +3250,27 @@
       </c>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="25">
-        <v>12273.93873354438</v>
+      <c r="B31" s="26">
+        <v>12051.8161047019</v>
       </c>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="27">
+      <c r="B32" s="28">
         <v>2795.73</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="29">
-        <v>4.390244670817417</v>
+      <c r="B33" s="30">
+        <v>4.310793998240852</v>
       </c>
     </row>
   </sheetData>
@@ -3268,7 +3281,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <tabColor rgb="FF93E100"/>
+    <tabColor rgb="FF96E100"/>
   </sheetPr>
   <dimension ref="A1:O33"/>
   <sheetViews>
@@ -3283,9 +3296,9 @@
   <cols>
     <col min="1" max="1" width="27.7109375" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
     <col min="4" max="13" width="14.7109375" customWidth="1"/>
-    <col min="14" max="14" width="6.7109375" customWidth="1"/>
+    <col min="14" max="14" width="5.7109375" customWidth="1"/>
     <col min="15" max="15" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3384,23 +3397,23 @@
         <v>0.26465</v>
       </c>
       <c r="I5" s="12">
-        <v>0.2233933335</v>
+        <v>0.2233933333333333</v>
       </c>
       <c r="J5" s="12">
-        <v>0.182136667</v>
+        <v>0.1821366666666667</v>
       </c>
       <c r="K5" s="12">
-        <v>0.1408800005</v>
+        <v>0.14088</v>
       </c>
       <c r="L5" s="12">
-        <v>0.09962333399999998</v>
+        <v>0.09962333333333334</v>
       </c>
       <c r="M5" s="13">
-        <v>0.05836666749999997</v>
+        <v>0.05836666666666668</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="10">
-        <v>0.017110001</v>
+        <v>0.01711</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -3427,23 +3440,23 @@
         <v>1656224322.007276</v>
       </c>
       <c r="I6" s="17">
-        <v>2026213794.324258</v>
+        <v>2026213794.048221</v>
       </c>
       <c r="J6" s="17">
-        <v>2395261621.451902</v>
+        <v>2395261620.450183</v>
       </c>
       <c r="K6" s="17">
-        <v>2732706079.879677</v>
+        <v>2732706077.539206</v>
       </c>
       <c r="L6" s="17">
-        <v>3004947370.39936</v>
+        <v>3004947366.00392</v>
       </c>
       <c r="M6" s="18">
-        <v>3180336134.422459</v>
+        <v>3180336127.266349</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="15">
-        <v>3234751688.862764</v>
+        <v>3234751678.403876</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -3513,23 +3526,23 @@
         <v>103957033.9920633</v>
       </c>
       <c r="I8" s="17">
-        <v>237623700.996952</v>
+        <v>237623700.9645798</v>
       </c>
       <c r="J8" s="17">
-        <v>411462833.77246</v>
+        <v>411462833.6003827</v>
       </c>
       <c r="K8" s="17">
-        <v>469429718.0000555</v>
+        <v>469429717.5980047</v>
       </c>
       <c r="L8" s="17">
-        <v>516195871.5859008</v>
+        <v>516195870.8308433</v>
       </c>
       <c r="M8" s="18">
-        <v>546324504.3876278</v>
+        <v>546324503.1583369</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="15">
-        <v>555672117.2040247</v>
+        <v>555672115.4073759</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -3599,23 +3612,23 @@
         <v>0</v>
       </c>
       <c r="I10" s="21">
-        <v>14070897.18867123</v>
+        <v>14070897.156299</v>
       </c>
       <c r="J10" s="21">
-        <v>411462833.77246</v>
+        <v>411462833.6003827</v>
       </c>
       <c r="K10" s="21">
-        <v>469429718.0000555</v>
+        <v>469429717.5980047</v>
       </c>
       <c r="L10" s="21">
-        <v>516195871.5859008</v>
+        <v>516195870.8308433</v>
       </c>
       <c r="M10" s="22">
-        <v>546324504.3876278</v>
+        <v>546324503.1583369</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="19">
-        <v>555672117.2040247</v>
+        <v>555672115.4073759</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -3685,23 +3698,23 @@
         <v>103957033.9920633</v>
       </c>
       <c r="I12" s="17">
-        <v>234246685.6716709</v>
+        <v>234246685.647068</v>
       </c>
       <c r="J12" s="17">
-        <v>312711753.6670696</v>
+        <v>312711753.5362908</v>
       </c>
       <c r="K12" s="17">
-        <v>356766585.6800421</v>
+        <v>356766585.3744836</v>
       </c>
       <c r="L12" s="17">
-        <v>392308862.4052846</v>
+        <v>392308861.8314409</v>
       </c>
       <c r="M12" s="18">
-        <v>415206623.3345972</v>
+        <v>415206622.400336</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="15">
-        <v>422310809.0750588</v>
+        <v>422310807.7096057</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -3771,23 +3784,23 @@
         <v>75753674.85386515</v>
       </c>
       <c r="I14" s="21">
-        <v>80867192.23228644</v>
+        <v>80867192.17195399</v>
       </c>
       <c r="J14" s="21">
-        <v>80661380.42346929</v>
+        <v>80661380.26485984</v>
       </c>
       <c r="K14" s="21">
-        <v>73753952.28548528</v>
+        <v>73753951.9928793</v>
       </c>
       <c r="L14" s="21">
-        <v>59502743.78390862</v>
+        <v>59502743.3347619</v>
       </c>
       <c r="M14" s="22">
-        <v>38334055.309249</v>
+        <v>38334054.70585981</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="19">
-        <v>11893400.84136386</v>
+        <v>11893400.11948828</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -3814,23 +3827,23 @@
         <v>28203359.1381982</v>
       </c>
       <c r="I15" s="17">
-        <v>153379493.4393845</v>
+        <v>153379493.475114</v>
       </c>
       <c r="J15" s="17">
-        <v>232050373.2436002</v>
+        <v>232050373.271431</v>
       </c>
       <c r="K15" s="17">
-        <v>283012633.3945569</v>
+        <v>283012633.3816043</v>
       </c>
       <c r="L15" s="17">
-        <v>332806118.621376</v>
+        <v>332806118.496679</v>
       </c>
       <c r="M15" s="18">
-        <v>376872568.0253482</v>
+        <v>376872567.6944762</v>
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="15">
-        <v>410417408.2336949</v>
+        <v>410417407.5901174</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -3842,38 +3855,38 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="11">
-        <v>0.06530571184897939</v>
+        <v>0.06628929678467285</v>
       </c>
       <c r="E16" s="12">
-        <v>0.06530571184897939</v>
+        <v>0.06628929678467285</v>
       </c>
       <c r="F16" s="12">
-        <v>0.06530571184897939</v>
+        <v>0.06628929678467285</v>
       </c>
       <c r="G16" s="12">
-        <v>0.06530571184897939</v>
+        <v>0.06628929678467285</v>
       </c>
       <c r="H16" s="12">
-        <v>0.06530571184897939</v>
+        <v>0.06628929678467285</v>
       </c>
       <c r="I16" s="12">
-        <v>0.06503940261156443</v>
+        <v>0.06594102205261679</v>
       </c>
       <c r="J16" s="12">
-        <v>0.06477309337414949</v>
+        <v>0.06559274732056071</v>
       </c>
       <c r="K16" s="12">
-        <v>0.06450678413673455</v>
+        <v>0.06524447258850463</v>
       </c>
       <c r="L16" s="12">
-        <v>0.0642404748993196</v>
+        <v>0.06489619785644857</v>
       </c>
       <c r="M16" s="13">
-        <v>0.06397416566190464</v>
+        <v>0.0645479231243925</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="10">
-        <v>0.0637078564244897</v>
+        <v>0.06419964839233643</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -3885,34 +3898,34 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="11">
-        <v>0.9386976798090825</v>
+        <v>0.9378317901299732</v>
       </c>
       <c r="E17" s="12">
-        <v>0.8811533340789547</v>
+        <v>0.87952846657839</v>
       </c>
       <c r="F17" s="12">
-        <v>0.8271365902559521</v>
+        <v>0.8248497562814818</v>
       </c>
       <c r="G17" s="12">
-        <v>0.776431198158458</v>
+        <v>0.7735703235217342</v>
       </c>
       <c r="H17" s="12">
-        <v>0.7288341642427304</v>
+        <v>0.7254788412998104</v>
       </c>
       <c r="I17" s="12">
-        <v>0.6843260093998109</v>
+        <v>0.6805994199405148</v>
       </c>
       <c r="J17" s="12">
-        <v>0.6426965647969716</v>
+        <v>0.6387050040007179</v>
       </c>
       <c r="K17" s="12">
-        <v>0.6037505578869266</v>
+        <v>0.5995853725940379</v>
       </c>
       <c r="L17" s="12">
-        <v>0.5673065177717876</v>
+        <v>0.5630458384591434</v>
       </c>
       <c r="M17" s="13">
-        <v>0.5331957636573468</v>
+        <v>0.528906051318604</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="10" t="s">
@@ -3928,42 +3941,43 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="16">
-        <v>-122168789.4755436</v>
+        <v>-122056096.4368885</v>
       </c>
       <c r="E18" s="17">
-        <v>-105700410.8026908</v>
+        <v>-105505496.7557625</v>
       </c>
       <c r="F18" s="17">
-        <v>-78790984.73708756</v>
+        <v>-78573146.59173</v>
       </c>
       <c r="G18" s="17">
-        <v>-38109616.59293164</v>
+        <v>-37969196.12066755</v>
       </c>
       <c r="H18" s="17">
-        <v>20555571.68632625</v>
+        <v>20460940.30834245</v>
       </c>
       <c r="I18" s="17">
-        <v>104961576.6691384</v>
+        <v>104389994.2899325</v>
       </c>
       <c r="J18" s="17">
-        <v>149137977.743517</v>
+        <v>148211734.5886974</v>
       </c>
       <c r="K18" s="17">
-        <v>170869035.3010119</v>
+        <v>169690235.2349291</v>
       </c>
       <c r="L18" s="17">
-        <v>188803080.2482373</v>
+        <v>187385100.0332957</v>
       </c>
       <c r="M18" s="18">
-        <v>200946856.7097809</v>
+        <v>199330181.6295887</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="15">
-        <v>4696199458.278621</v>
+        <v>4609765794.646161</v>
       </c>
     </row>
     <row r="20" spans="1:15">
-      <c r="B20" s="23" t="s">
+      <c r="A20" s="23"/>
+      <c r="B20" s="24" t="s">
         <v>4</v>
       </c>
     </row>
@@ -3972,7 +3986,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="19">
-        <v>490504296.7497582</v>
+        <v>485364250.1797373</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -3980,7 +3994,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="19">
-        <v>4696199458.278621</v>
+        <v>4609765794.646161</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -3988,7 +4002,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="15">
-        <v>5186703755.028379</v>
+        <v>5095130044.825898</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -4028,7 +4042,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="15">
-        <v>5452940747.028379</v>
+        <v>5361367036.825898</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -4048,27 +4062,27 @@
       </c>
     </row>
     <row r="31" spans="1:15">
-      <c r="A31" s="24" t="s">
+      <c r="A31" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="25">
-        <v>57.9300792284337</v>
+      <c r="B31" s="26">
+        <v>56.95723310129354</v>
       </c>
     </row>
     <row r="32" spans="1:15">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="27" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="27">
+      <c r="B32" s="28">
         <v>34.27</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="28" t="s">
+      <c r="A33" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="29">
-        <v>1.690402078448605</v>
+      <c r="B33" s="30">
+        <v>1.66201438871589</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
simplified valuation tool methods to make assumptions adjustments all in the same method; updated README
</commit_message>
<xml_diff>
--- a/DCF valuations.xlsx
+++ b/DCF valuations.xlsx
@@ -19,7 +19,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="36">
   <si>
-    <t>Valuation of Asana, Inc. on 2022-01-18</t>
+    <t>Valuation of Asana, Inc. on 2022-01-19</t>
   </si>
   <si>
     <t>Year Ended</t>
@@ -58,7 +58,7 @@
     <t>After-Tax Operating Income</t>
   </si>
   <si>
-    <t>Sales to Capital</t>
+    <t>Sales-to-Capital Ratio</t>
   </si>
   <si>
     <t>Reinvestment</t>
@@ -118,13 +118,13 @@
     <t>--</t>
   </si>
   <si>
-    <t>Valuation of Salesforce.com Inc on 2022-01-18</t>
+    <t>Valuation of Salesforce.com Inc on 2022-01-19</t>
   </si>
   <si>
-    <t>Valuation of Alphabet Inc. on 2022-01-18</t>
+    <t>Valuation of Alphabet Inc. on 2022-01-19</t>
   </si>
   <si>
-    <t>Valuation of Warby Parker Inc. on 2022-01-18</t>
+    <t>Valuation of Warby Parker Inc. on 2022-01-19</t>
   </si>
 </sst>
 </file>
@@ -845,7 +845,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <tabColor rgb="FFE18D00"/>
+    <tabColor rgb="FFE1A900"/>
   </sheetPr>
   <dimension ref="A1:O33"/>
   <sheetViews>
@@ -961,23 +961,23 @@
         <v>0.5610999999999999</v>
       </c>
       <c r="I5" s="12">
-        <v>0.4704349999999999</v>
+        <v>0.4706916666666666</v>
       </c>
       <c r="J5" s="12">
-        <v>0.3797699999999999</v>
+        <v>0.3802833333333333</v>
       </c>
       <c r="K5" s="12">
-        <v>0.2891049999999999</v>
+        <v>0.289875</v>
       </c>
       <c r="L5" s="12">
-        <v>0.1984399999999999</v>
+        <v>0.1994666666666667</v>
       </c>
       <c r="M5" s="13">
-        <v>0.107775</v>
+        <v>0.1090583333333334</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="10">
-        <v>0.01711</v>
+        <v>0.01865</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1004,23 +1004,23 @@
         <v>3104652525.092923</v>
       </c>
       <c r="I6" s="17">
-        <v>4565189735.735011</v>
+        <v>4565986596.549786</v>
       </c>
       <c r="J6" s="17">
-        <v>6298911841.675096</v>
+        <v>6302355199.44106</v>
       </c>
       <c r="K6" s="17">
-        <v>8119958749.662574</v>
+        <v>8129250412.879037</v>
       </c>
       <c r="L6" s="17">
-        <v>9731283363.945614</v>
+        <v>9750764895.234642</v>
       </c>
       <c r="M6" s="18">
-        <v>10780072428.49485</v>
+        <v>10814167063.43411</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="15">
-        <v>10964519467.7464</v>
+        <v>11015851279.16716</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1090,23 +1090,23 @@
         <v>-722451400.3353819</v>
       </c>
       <c r="I8" s="17">
-        <v>-650146700.6204185</v>
+        <v>-650260184.7162764</v>
       </c>
       <c r="J8" s="17">
-        <v>-328351561.0338088</v>
+        <v>-328531057.41764</v>
       </c>
       <c r="K8" s="17">
-        <v>309836117.38818</v>
+        <v>310190662.6443596</v>
       </c>
       <c r="L8" s="17">
-        <v>1249915243.712191</v>
+        <v>1252417510.06477</v>
       </c>
       <c r="M8" s="18">
-        <v>1384624859.103273</v>
+        <v>1389004076.349918</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="15">
-        <v>1408315790.44253</v>
+        <v>1414909002.373844</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1136,20 +1136,20 @@
         <v>2841721219.956268</v>
       </c>
       <c r="J9" s="21">
-        <v>3491867920.576686</v>
+        <v>3491981404.672544</v>
       </c>
       <c r="K9" s="21">
-        <v>3820219481.610495</v>
+        <v>3820512462.090185</v>
       </c>
       <c r="L9" s="21">
-        <v>3510383364.222315</v>
+        <v>3510321799.445825</v>
       </c>
       <c r="M9" s="22">
-        <v>2260468120.510124</v>
+        <v>2257904289.381055</v>
       </c>
       <c r="N9" s="6"/>
       <c r="O9" s="19">
-        <v>875843261.4068515</v>
+        <v>868900213.0311372</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -1192,7 +1192,7 @@
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="19">
-        <v>532472529.0356781</v>
+        <v>546008789.3427067</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1200,42 +1200,42 @@
         <v>11</v>
       </c>
       <c r="B11" s="10">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="11">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="E11" s="12">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="F11" s="12">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="G11" s="12">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="H11" s="12">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="I11" s="12">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="J11" s="12">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="K11" s="12">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="L11" s="12">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="M11" s="13">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
       <c r="N11" s="6"/>
       <c r="O11" s="10">
-        <v>0.24</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1262,23 +1262,23 @@
         <v>-722451400.3353819</v>
       </c>
       <c r="I12" s="17">
-        <v>-650146700.6204185</v>
+        <v>-650260184.7162764</v>
       </c>
       <c r="J12" s="17">
-        <v>-328351561.0338088</v>
+        <v>-328531057.41764</v>
       </c>
       <c r="K12" s="17">
-        <v>309836117.38818</v>
+        <v>310190662.6443596</v>
       </c>
       <c r="L12" s="17">
-        <v>1249915243.712191</v>
+        <v>1252417510.06477</v>
       </c>
       <c r="M12" s="18">
-        <v>1384624859.103273</v>
+        <v>1389004076.349918</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="15">
-        <v>1280522383.473967</v>
+        <v>1300247156.611876</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1348,23 +1348,23 @@
         <v>884270596.9261782</v>
       </c>
       <c r="I14" s="21">
-        <v>1157378112.128746</v>
+        <v>1158009571.059551</v>
       </c>
       <c r="J14" s="21">
-        <v>1373858881.039169</v>
+        <v>1375956052.972074</v>
       </c>
       <c r="K14" s="21">
-        <v>1443057949.573134</v>
+        <v>1447692340.721905</v>
       </c>
       <c r="L14" s="21">
-        <v>1276867050.368147</v>
+        <v>1284941839.690003</v>
       </c>
       <c r="M14" s="22">
-        <v>831095229.0052466</v>
+        <v>842675136.8581988</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="19">
-        <v>146161949.5355706</v>
+        <v>159821259.7052983</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1391,23 +1391,23 @@
         <v>-1606721997.26156</v>
       </c>
       <c r="I15" s="17">
-        <v>-1807524812.749164</v>
+        <v>-1808269755.775827</v>
       </c>
       <c r="J15" s="17">
-        <v>-1702210442.072978</v>
+        <v>-1704487110.389714</v>
       </c>
       <c r="K15" s="17">
-        <v>-1133221832.184954</v>
+        <v>-1137501678.077546</v>
       </c>
       <c r="L15" s="17">
-        <v>-26951806.65595555</v>
+        <v>-32524329.6252327</v>
       </c>
       <c r="M15" s="18">
-        <v>553529630.098026</v>
+        <v>546328939.4917189</v>
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="15">
-        <v>1134360433.938396</v>
+        <v>1140425896.906577</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1419,38 +1419,38 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="11">
-        <v>0.07628218674670335</v>
+        <v>0.07800495571685999</v>
       </c>
       <c r="E16" s="12">
-        <v>0.07628218674670335</v>
+        <v>0.07800495571685999</v>
       </c>
       <c r="F16" s="12">
-        <v>0.07628218674670335</v>
+        <v>0.07800495571685999</v>
       </c>
       <c r="G16" s="12">
-        <v>0.07628218674670335</v>
+        <v>0.07800495571685999</v>
       </c>
       <c r="H16" s="12">
-        <v>0.07628218674670335</v>
+        <v>0.07800495571685999</v>
       </c>
       <c r="I16" s="12">
-        <v>0.07510117118447807</v>
+        <v>0.07680870940712166</v>
       </c>
       <c r="J16" s="12">
-        <v>0.07392015562225279</v>
+        <v>0.07561246309738333</v>
       </c>
       <c r="K16" s="12">
-        <v>0.07273914006002752</v>
+        <v>0.07441621678764498</v>
       </c>
       <c r="L16" s="12">
-        <v>0.07155812449780223</v>
+        <v>0.07321997047790665</v>
       </c>
       <c r="M16" s="13">
-        <v>0.07037710893557694</v>
+        <v>0.07202372416816832</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="10">
-        <v>0.06919609337335167</v>
+        <v>0.07082747785842999</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1462,34 +1462,34 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="11">
-        <v>0.9291243619135955</v>
+        <v>0.9276395202979492</v>
       </c>
       <c r="E17" s="12">
-        <v>0.8632720799013459</v>
+        <v>0.8605150796186093</v>
       </c>
       <c r="F17" s="12">
-        <v>0.8020871203961605</v>
+        <v>0.7982477956665582</v>
       </c>
       <c r="G17" s="12">
-        <v>0.7452386839371958</v>
+        <v>0.7404862022510215</v>
       </c>
       <c r="H17" s="12">
-        <v>0.6924194166864748</v>
+        <v>0.6869042654433877</v>
       </c>
       <c r="I17" s="12">
-        <v>0.6440504719417347</v>
+        <v>0.6379074198068003</v>
       </c>
       <c r="J17" s="12">
-        <v>0.5997191397982076</v>
+        <v>0.5930643625770685</v>
       </c>
       <c r="K17" s="12">
-        <v>0.5590540303811875</v>
+        <v>0.5519875382654298</v>
       </c>
       <c r="L17" s="12">
-        <v>0.521720677208429</v>
+        <v>0.5143284260910919</v>
       </c>
       <c r="M17" s="13">
-        <v>0.4874176333304134</v>
+        <v>0.4797733618163932</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="10" t="s">
@@ -1505,38 +1505,38 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="16">
-        <v>-426762694.9925799</v>
+        <v>-426080681.8676359</v>
       </c>
       <c r="E18" s="17">
-        <v>-555396115.2513537</v>
+        <v>-553622367.1104968</v>
       </c>
       <c r="F18" s="17">
-        <v>-713322244.2726279</v>
+        <v>-709907807.5325658</v>
       </c>
       <c r="G18" s="17">
-        <v>-900830147.0161034</v>
+        <v>-895085438.8194895</v>
       </c>
       <c r="H18" s="17">
-        <v>-1112525508.121177</v>
+        <v>-1103664193.300685</v>
       </c>
       <c r="I18" s="17">
-        <v>-1164137208.697495</v>
+        <v>-1153508694.221631</v>
       </c>
       <c r="J18" s="17">
-        <v>-1020848182.075533</v>
+        <v>-1010870561.644105</v>
       </c>
       <c r="K18" s="17">
-        <v>-633532232.5989524</v>
+        <v>-627886751.0548199</v>
       </c>
       <c r="L18" s="17">
-        <v>-14061314.82053577</v>
+        <v>-16728187.26581381</v>
       </c>
       <c r="M18" s="18">
-        <v>269800102.280639</v>
+        <v>262114071.9575268</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="15">
-        <v>10615257206.76899</v>
+        <v>10486247877.789</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1550,7 +1550,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="19">
-        <v>-6271615545.565719</v>
+        <v>-6235240610.859715</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1558,7 +1558,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="19">
-        <v>10615257206.76899</v>
+        <v>10486247877.789</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1566,7 +1566,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="15">
-        <v>4343641661.203271</v>
+        <v>4251007266.929282</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1606,7 +1606,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="15">
-        <v>4431947661.203271</v>
+        <v>4339313266.929282</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -1614,7 +1614,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="19">
-        <v>11219297280</v>
+        <v>9919886336</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -1630,7 +1630,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="26">
-        <v>45.36727929462128</v>
+        <v>44.41903469459929</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -1638,7 +1638,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="28">
-        <v>60.18</v>
+        <v>53.21</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1646,7 +1646,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="30">
-        <v>0.7538597423499714</v>
+        <v>0.8347873462619675</v>
       </c>
     </row>
   </sheetData>
@@ -1773,23 +1773,23 @@
         <v>0.2546410854503579</v>
       </c>
       <c r="I5" s="12">
-        <v>0.2150525712086316</v>
+        <v>0.2153092378752983</v>
       </c>
       <c r="J5" s="12">
-        <v>0.1754640569669053</v>
+        <v>0.1759773903002386</v>
       </c>
       <c r="K5" s="12">
-        <v>0.135875542725179</v>
+        <v>0.136645542725179</v>
       </c>
       <c r="L5" s="12">
-        <v>0.09628702848345264</v>
+        <v>0.09731369515011931</v>
       </c>
       <c r="M5" s="13">
-        <v>0.05669851424172631</v>
+        <v>0.05798184757505967</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="10">
-        <v>0.01711</v>
+        <v>0.01865</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -1816,23 +1816,23 @@
         <v>77667998554.88492</v>
       </c>
       <c r="I6" s="17">
-        <v>94370701344.7412</v>
+        <v>94390636131.03696</v>
       </c>
       <c r="J6" s="17">
-        <v>110929367461.5017</v>
+        <v>111001253946.1562</v>
       </c>
       <c r="K6" s="17">
-        <v>126001955469.494</v>
+        <v>126169080534.8042</v>
       </c>
       <c r="L6" s="17">
-        <v>138134309344.7559</v>
+        <v>138447059975.339</v>
       </c>
       <c r="M6" s="18">
-        <v>145966319450.4106</v>
+        <v>146474476304.0442</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="15">
-        <v>148463803176.2071</v>
+        <v>149206225287.1147</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1902,23 +1902,23 @@
         <v>8816372006.531195</v>
       </c>
       <c r="I8" s="17">
-        <v>12121256134.37864</v>
+        <v>12123816618.16473</v>
       </c>
       <c r="J8" s="17">
-        <v>14248100911.25171</v>
+        <v>14257334227.10803</v>
       </c>
       <c r="K8" s="17">
-        <v>16184069355.37115</v>
+        <v>16205535400.38547</v>
       </c>
       <c r="L8" s="17">
-        <v>17742385302.36995</v>
+        <v>17782555932.08305</v>
       </c>
       <c r="M8" s="18">
-        <v>18748352188.11856</v>
+        <v>18813621379.63206</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="15">
-        <v>19069136494.05727</v>
+        <v>19164495418.3622</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1988,23 +1988,23 @@
         <v>8816372006.531195</v>
       </c>
       <c r="I10" s="21">
-        <v>12121256134.37864</v>
+        <v>12123816618.16473</v>
       </c>
       <c r="J10" s="21">
-        <v>14248100911.25171</v>
+        <v>14257334227.10803</v>
       </c>
       <c r="K10" s="21">
-        <v>16184069355.37115</v>
+        <v>16205535400.38547</v>
       </c>
       <c r="L10" s="21">
-        <v>17742385302.36995</v>
+        <v>17782555932.08305</v>
       </c>
       <c r="M10" s="22">
-        <v>18748352188.11856</v>
+        <v>18813621379.63206</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="19">
-        <v>19069136494.05727</v>
+        <v>19164495418.3622</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -2074,23 +2074,23 @@
         <v>6700442724.963708</v>
       </c>
       <c r="I12" s="17">
-        <v>9212154662.127769</v>
+        <v>9214100629.805197</v>
       </c>
       <c r="J12" s="17">
-        <v>10828556692.5513</v>
+        <v>10835574012.6021</v>
       </c>
       <c r="K12" s="17">
-        <v>12299892710.08208</v>
+        <v>12316206904.29296</v>
       </c>
       <c r="L12" s="17">
-        <v>13484212829.80116</v>
+        <v>13514742508.38312</v>
       </c>
       <c r="M12" s="18">
-        <v>14248747662.97011</v>
+        <v>14298352248.52037</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="15">
-        <v>14492543735.48352</v>
+        <v>14565016517.95527</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -2160,23 +2160,23 @@
         <v>18272548994.35591</v>
       </c>
       <c r="I14" s="21">
-        <v>19361312859.01226</v>
+        <v>19384420714.01668</v>
       </c>
       <c r="J14" s="21">
-        <v>19194349516.24879</v>
+        <v>19254570493.54434</v>
       </c>
       <c r="K14" s="21">
-        <v>17471728718.95708</v>
+        <v>17582126657.51351</v>
       </c>
       <c r="L14" s="21">
-        <v>14063490325.52095</v>
+        <v>14232295468.31682</v>
       </c>
       <c r="M14" s="22">
-        <v>9078650316.559362</v>
+        <v>9305159826.228554</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="19">
-        <v>2895014320.963912</v>
+        <v>3166568152.409206</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -2203,23 +2203,23 @@
         <v>-11572106269.3922</v>
       </c>
       <c r="I15" s="17">
-        <v>-10149158196.88449</v>
+        <v>-10170320084.21148</v>
       </c>
       <c r="J15" s="17">
-        <v>-8365792823.697493</v>
+        <v>-8418996480.942238</v>
       </c>
       <c r="K15" s="17">
-        <v>-5171836008.875006</v>
+        <v>-5265919753.220552</v>
       </c>
       <c r="L15" s="17">
-        <v>-579277495.7197914</v>
+        <v>-717552959.9336987</v>
       </c>
       <c r="M15" s="18">
-        <v>5170097346.410746</v>
+        <v>4993192422.291817</v>
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="15">
-        <v>11597529414.51961</v>
+        <v>11398448365.54607</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -2231,38 +2231,38 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="11">
-        <v>0.07598471660702244</v>
+        <v>0.07750517682891413</v>
       </c>
       <c r="E16" s="12">
-        <v>0.07598471660702244</v>
+        <v>0.07750517682891413</v>
       </c>
       <c r="F16" s="12">
-        <v>0.07598471660702244</v>
+        <v>0.07750517682891413</v>
       </c>
       <c r="G16" s="12">
-        <v>0.07598471660702244</v>
+        <v>0.07750517682891413</v>
       </c>
       <c r="H16" s="12">
-        <v>0.07598471660702244</v>
+        <v>0.07750517682891413</v>
       </c>
       <c r="I16" s="12">
-        <v>0.07482849022310391</v>
+        <v>0.07635057875983794</v>
       </c>
       <c r="J16" s="12">
-        <v>0.07367226383918536</v>
+        <v>0.07519598069076178</v>
       </c>
       <c r="K16" s="12">
-        <v>0.07251603745526683</v>
+        <v>0.07404138262168559</v>
       </c>
       <c r="L16" s="12">
-        <v>0.0713598110713483</v>
+        <v>0.07288678455260941</v>
       </c>
       <c r="M16" s="13">
-        <v>0.07020358468742975</v>
+        <v>0.07173218648353324</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="10">
-        <v>0.06904735830351122</v>
+        <v>0.07057758841445706</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -2274,34 +2274,34 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="11">
-        <v>0.9293812305748819</v>
+        <v>0.9280697870454683</v>
       </c>
       <c r="E17" s="12">
-        <v>0.8637494717448817</v>
+        <v>0.8613135296266209</v>
       </c>
       <c r="F17" s="12">
-        <v>0.8027525469586623</v>
+        <v>0.7993590640199587</v>
       </c>
       <c r="G17" s="12">
-        <v>0.7460631499395621</v>
+        <v>0.7418609963178679</v>
       </c>
       <c r="H17" s="12">
-        <v>0.6933770883774029</v>
+        <v>0.6884987768700627</v>
       </c>
       <c r="I17" s="12">
-        <v>0.6451048652734144</v>
+        <v>0.6396603397225327</v>
       </c>
       <c r="J17" s="12">
-        <v>0.6008396481871289</v>
+        <v>0.5949244149067425</v>
       </c>
       <c r="K17" s="12">
-        <v>0.5602150711076794</v>
+        <v>0.5539120042605429</v>
       </c>
       <c r="L17" s="12">
-        <v>0.5229009575666931</v>
+        <v>0.5162818782333334</v>
       </c>
       <c r="M17" s="13">
-        <v>0.4885995198001647</v>
+        <v>0.4817265775392161</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="10" t="s">
@@ -2317,38 +2317,38 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="16">
-        <v>-5662517198.331181</v>
+        <v>-5654526858.84977</v>
       </c>
       <c r="E18" s="17">
-        <v>-6217306240.040591</v>
+        <v>-6199772222.796394</v>
       </c>
       <c r="F18" s="17">
-        <v>-6800218191.155452</v>
+        <v>-6771471568.676861</v>
       </c>
       <c r="G18" s="17">
-        <v>-7405296987.991713</v>
+        <v>-7363587119.919108</v>
       </c>
       <c r="H18" s="17">
-        <v>-8023833351.465054</v>
+        <v>-7967381012.286914</v>
       </c>
       <c r="I18" s="17">
-        <v>-6547271331.239741</v>
+        <v>-6505550400.153613</v>
       </c>
       <c r="J18" s="17">
-        <v>-5026500016.996809</v>
+        <v>-5008666555.526485</v>
       </c>
       <c r="K18" s="17">
-        <v>-2897340477.469168</v>
+        <v>-2916856164.781579</v>
       </c>
       <c r="L18" s="17">
-        <v>-302904757.2087149</v>
+        <v>-370459589.8864577</v>
       </c>
       <c r="M18" s="18">
-        <v>2526107080.776396</v>
+        <v>2405353496.585385</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="15">
-        <v>109103494823.2914</v>
+        <v>105742163039.9315</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -2362,7 +2362,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="19">
-        <v>-46357081471.12202</v>
+        <v>-46352917996.2918</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -2370,7 +2370,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="19">
-        <v>109103494823.2914</v>
+        <v>105742163039.9315</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -2378,7 +2378,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="15">
-        <v>62746413352.16937</v>
+        <v>59389245043.63973</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -2418,7 +2418,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="15">
-        <v>57799413032.16937</v>
+        <v>54442244723.63974</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -2426,7 +2426,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="19">
-        <v>227761553408</v>
+        <v>222669094912</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -2442,7 +2442,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="26">
-        <v>58.67960713925824</v>
+        <v>55.27131444024339</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -2450,7 +2450,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="28">
-        <v>231.23</v>
+        <v>226.06</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -2458,7 +2458,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="30">
-        <v>0.2537716003081704</v>
+        <v>0.244498427144313</v>
       </c>
     </row>
   </sheetData>
@@ -2585,23 +2585,23 @@
         <v>0.3201761451922981</v>
       </c>
       <c r="I5" s="12">
-        <v>0.2696651209935818</v>
+        <v>0.2699217876602484</v>
       </c>
       <c r="J5" s="12">
-        <v>0.2191540967948654</v>
+        <v>0.2196674301281987</v>
       </c>
       <c r="K5" s="12">
-        <v>0.1686430725961491</v>
+        <v>0.169413072596149</v>
       </c>
       <c r="L5" s="12">
-        <v>0.1181320483974327</v>
+        <v>0.1191587150640994</v>
       </c>
       <c r="M5" s="13">
-        <v>0.06762102419871635</v>
+        <v>0.06890435753204971</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="10">
-        <v>0.01711</v>
+        <v>0.01865</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -2628,23 +2628,23 @@
         <v>959265303239.4132</v>
       </c>
       <c r="I6" s="17">
-        <v>1217945697302.414</v>
+        <v>1218191908730.246</v>
       </c>
       <c r="J6" s="17">
-        <v>1484863486539.917</v>
+        <v>1485788994723.984</v>
       </c>
       <c r="K6" s="17">
-        <v>1735275427295.84</v>
+        <v>1737501073549.718</v>
       </c>
       <c r="L6" s="17">
-        <v>1940267068056.027</v>
+        <v>1944539468896.395</v>
       </c>
       <c r="M6" s="18">
-        <v>2071469914417.016</v>
+        <v>2078526711696.414</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="15">
-        <v>2106912764652.691</v>
+        <v>2117291234869.552</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -2714,23 +2714,23 @@
         <v>222274179164.1181</v>
       </c>
       <c r="I8" s="17">
-        <v>282213772582.159</v>
+        <v>282270822954.8112</v>
       </c>
       <c r="J8" s="17">
-        <v>344062077015.4736</v>
+        <v>344276529233.4662</v>
       </c>
       <c r="K8" s="17">
-        <v>402085762847.1759</v>
+        <v>402601473873.6458</v>
       </c>
       <c r="L8" s="17">
-        <v>449584977643.7571</v>
+        <v>450574948183.3419</v>
       </c>
       <c r="M8" s="18">
-        <v>479986374296.385</v>
+        <v>481621525507.9516</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="15">
-        <v>488198941160.5961</v>
+        <v>490603766958.6749</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -2800,23 +2800,23 @@
         <v>222274179164.1181</v>
       </c>
       <c r="I10" s="21">
-        <v>282213772582.159</v>
+        <v>282270822954.8112</v>
       </c>
       <c r="J10" s="21">
-        <v>344062077015.4736</v>
+        <v>344276529233.4662</v>
       </c>
       <c r="K10" s="21">
-        <v>402085762847.1759</v>
+        <v>402601473873.6458</v>
       </c>
       <c r="L10" s="21">
-        <v>449584977643.7571</v>
+        <v>450574948183.3419</v>
       </c>
       <c r="M10" s="22">
-        <v>479986374296.385</v>
+        <v>481621525507.9516</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="19">
-        <v>488198941160.5961</v>
+        <v>490603766958.6749</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -2886,23 +2886,23 @@
         <v>168928376164.7297</v>
       </c>
       <c r="I12" s="17">
-        <v>214482467162.4409</v>
+        <v>214525825445.6565</v>
       </c>
       <c r="J12" s="17">
-        <v>261487178531.7599</v>
+        <v>261650162217.4344</v>
       </c>
       <c r="K12" s="17">
-        <v>305585179763.8537</v>
+        <v>305977120143.9708</v>
       </c>
       <c r="L12" s="17">
-        <v>341684583009.2554</v>
+        <v>342436960619.3398</v>
       </c>
       <c r="M12" s="18">
-        <v>364789644465.2526</v>
+        <v>366032359386.0432</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="15">
-        <v>371031195282.0531</v>
+        <v>372858862888.593</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -2972,23 +2972,23 @@
         <v>209239330509.4904</v>
       </c>
       <c r="I14" s="21">
-        <v>232654259885.3698</v>
+        <v>232875699696.164</v>
       </c>
       <c r="J14" s="21">
-        <v>240062881186.7598</v>
+        <v>240673833109.2542</v>
       </c>
       <c r="K14" s="21">
-        <v>225217705246.1083</v>
+        <v>226387034918.2563</v>
       </c>
       <c r="L14" s="21">
-        <v>184367194261.0918</v>
+        <v>186208022497.0762</v>
       </c>
       <c r="M14" s="22">
-        <v>118002375964.8963</v>
+        <v>120506631051.9371</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="19">
-        <v>31876904006.10997</v>
+        <v>34864379580.53844</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -3015,23 +3015,23 @@
         <v>-40310954344.76071</v>
       </c>
       <c r="I15" s="17">
-        <v>-18171792722.92899</v>
+        <v>-18349874250.50748</v>
       </c>
       <c r="J15" s="17">
-        <v>21424297345.00015</v>
+        <v>20976329108.18011</v>
       </c>
       <c r="K15" s="17">
-        <v>80367474517.74536</v>
+        <v>79590085225.71445</v>
       </c>
       <c r="L15" s="17">
-        <v>157317388748.1637</v>
+        <v>156228938122.2636</v>
       </c>
       <c r="M15" s="18">
-        <v>246787268500.3563</v>
+        <v>245525728334.1061</v>
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="15">
-        <v>339154291275.9431</v>
+        <v>337994483308.0545</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -3043,38 +3043,38 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="11">
-        <v>0.0706354870011382</v>
+        <v>0.07217774574901543</v>
       </c>
       <c r="E16" s="12">
-        <v>0.0706354870011382</v>
+        <v>0.07217774574901543</v>
       </c>
       <c r="F16" s="12">
-        <v>0.0706354870011382</v>
+        <v>0.07217774574901543</v>
       </c>
       <c r="G16" s="12">
-        <v>0.0706354870011382</v>
+        <v>0.07217774574901543</v>
       </c>
       <c r="H16" s="12">
-        <v>0.0706354870011382</v>
+        <v>0.07217774574901543</v>
       </c>
       <c r="I16" s="12">
-        <v>0.06992502975104335</v>
+        <v>0.07146710026993082</v>
       </c>
       <c r="J16" s="12">
-        <v>0.06921457250094849</v>
+        <v>0.07075645479084619</v>
       </c>
       <c r="K16" s="12">
-        <v>0.06850411525085365</v>
+        <v>0.07004580931176158</v>
       </c>
       <c r="L16" s="12">
-        <v>0.0677936580007588</v>
+        <v>0.06933516383267696</v>
       </c>
       <c r="M16" s="13">
-        <v>0.06708320075066394</v>
+        <v>0.06862451835359233</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="10">
-        <v>0.0663727435005691</v>
+        <v>0.06791387287450772</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -3086,34 +3086,34 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="11">
-        <v>0.934024709755335</v>
+        <v>0.9326811752667068</v>
       </c>
       <c r="E17" s="12">
-        <v>0.8724021584335379</v>
+        <v>0.8698941746968855</v>
       </c>
       <c r="F17" s="12">
-        <v>0.814845172820813</v>
+        <v>0.8113339212139531</v>
       </c>
       <c r="G17" s="12">
-        <v>0.7610855260394958</v>
+        <v>0.7567158751715755</v>
       </c>
       <c r="H17" s="12">
-        <v>0.7108726875580265</v>
+        <v>0.7057746517979996</v>
       </c>
       <c r="I17" s="12">
-        <v>0.6644135502871977</v>
+        <v>0.6586993213512542</v>
       </c>
       <c r="J17" s="12">
-        <v>0.6214033809257761</v>
+        <v>0.6151719360682442</v>
       </c>
       <c r="K17" s="12">
-        <v>0.5815638630272272</v>
+        <v>0.5749024300781236</v>
       </c>
       <c r="L17" s="12">
-        <v>0.5446406790953369</v>
+        <v>0.5376260404806821</v>
       </c>
       <c r="M17" s="13">
-        <v>0.510401324575438</v>
+        <v>0.5031009781705097</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="10" t="s">
@@ -3129,38 +3129,38 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="16">
-        <v>388820936.7219916</v>
+        <v>388261642.8051063</v>
       </c>
       <c r="E18" s="17">
-        <v>-3461478156.484266</v>
+        <v>-3451527091.098518</v>
       </c>
       <c r="F18" s="17">
-        <v>-9127733337.069708</v>
+        <v>-9088400995.889082</v>
       </c>
       <c r="G18" s="17">
-        <v>-17247292990.99172</v>
+        <v>-17148270415.72407</v>
       </c>
       <c r="H18" s="17">
-        <v>-28655956453.08895</v>
+        <v>-28450449766.31855</v>
       </c>
       <c r="I18" s="17">
-        <v>-12073585318.12431</v>
+        <v>-12087049715.69013</v>
       </c>
       <c r="J18" s="17">
-        <v>13313130804.14222</v>
+        <v>12904048989.08383</v>
       </c>
       <c r="K18" s="17">
-        <v>46738818942.28223</v>
+        <v>45756533406.3882</v>
       </c>
       <c r="L18" s="17">
-        <v>85681449441.30496</v>
+        <v>83992745411.17409</v>
       </c>
       <c r="M18" s="18">
-        <v>125960548730.9361</v>
+        <v>123524234090.9156</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="15">
-        <v>3513909035551.086</v>
+        <v>3451725275470.792</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -3174,7 +3174,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="19">
-        <v>201516722599.6286</v>
+        <v>196340125555.6465</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -3182,7 +3182,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="19">
-        <v>3513909035551.086</v>
+        <v>3451725275470.792</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -3190,7 +3190,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="15">
-        <v>3715425758150.714</v>
+        <v>3648065401026.438</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -3230,7 +3230,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="15">
-        <v>3829319752646.714</v>
+        <v>3761959395522.438</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -3238,7 +3238,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="19">
-        <v>1853588504576</v>
+        <v>1807269232640</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -3254,7 +3254,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="26">
-        <v>12051.8161047019</v>
+        <v>11839.81640521279</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -3262,7 +3262,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="28">
-        <v>2795.73</v>
+        <v>2725.81</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -3270,7 +3270,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="30">
-        <v>4.310793998240852</v>
+        <v>4.343595630367776</v>
       </c>
     </row>
   </sheetData>
@@ -3281,7 +3281,7 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <tabColor rgb="FF96E100"/>
+    <tabColor rgb="FFE10000"/>
   </sheetPr>
   <dimension ref="A1:O33"/>
   <sheetViews>
@@ -3397,23 +3397,23 @@
         <v>0.26465</v>
       </c>
       <c r="I5" s="12">
-        <v>0.2233933333333333</v>
+        <v>0.22365</v>
       </c>
       <c r="J5" s="12">
-        <v>0.1821366666666667</v>
+        <v>0.18265</v>
       </c>
       <c r="K5" s="12">
-        <v>0.14088</v>
+        <v>0.14165</v>
       </c>
       <c r="L5" s="12">
-        <v>0.09962333333333334</v>
+        <v>0.10065</v>
       </c>
       <c r="M5" s="13">
-        <v>0.05836666666666668</v>
+        <v>0.05964999999999998</v>
       </c>
       <c r="N5" s="6"/>
       <c r="O5" s="10">
-        <v>0.01711</v>
+        <v>0.01865</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -3440,23 +3440,23 @@
         <v>1656224322.007276</v>
       </c>
       <c r="I6" s="17">
-        <v>2026213794.048221</v>
+        <v>2026638891.624202</v>
       </c>
       <c r="J6" s="17">
-        <v>2395261620.450183</v>
+        <v>2396804485.179363</v>
       </c>
       <c r="K6" s="17">
-        <v>2732706077.539206</v>
+        <v>2736311840.50502</v>
       </c>
       <c r="L6" s="17">
-        <v>3004947366.00392</v>
+        <v>3011721627.25185</v>
       </c>
       <c r="M6" s="18">
-        <v>3180336127.266349</v>
+        <v>3191370822.317423</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="15">
-        <v>3234751678.403876</v>
+        <v>3250889888.153643</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -3526,23 +3526,23 @@
         <v>103957033.9920633</v>
       </c>
       <c r="I8" s="17">
-        <v>237623700.9645798</v>
+        <v>237673554.1733441</v>
       </c>
       <c r="J8" s="17">
-        <v>411462833.6003827</v>
+        <v>411727869.9905249</v>
       </c>
       <c r="K8" s="17">
-        <v>469429717.5980047</v>
+        <v>470049122.7746828</v>
       </c>
       <c r="L8" s="17">
-        <v>516195870.8308433</v>
+        <v>517359566.9819546</v>
       </c>
       <c r="M8" s="18">
-        <v>546324503.1583369</v>
+        <v>548220065.1524282</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="15">
-        <v>555672115.4073759</v>
+        <v>558444369.367521</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -3612,23 +3612,23 @@
         <v>0</v>
       </c>
       <c r="I10" s="21">
-        <v>14070897.156299</v>
+        <v>14120750.36506331</v>
       </c>
       <c r="J10" s="21">
-        <v>411462833.6003827</v>
+        <v>411727869.9905249</v>
       </c>
       <c r="K10" s="21">
-        <v>469429717.5980047</v>
+        <v>470049122.7746828</v>
       </c>
       <c r="L10" s="21">
-        <v>516195870.8308433</v>
+        <v>517359566.9819546</v>
       </c>
       <c r="M10" s="22">
-        <v>546324503.1583369</v>
+        <v>548220065.1524282</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="19">
-        <v>555672115.4073759</v>
+        <v>558444369.367521</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -3636,42 +3636,42 @@
         <v>11</v>
       </c>
       <c r="B11" s="10">
-        <v>0.24</v>
+        <v>1</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="11">
-        <v>0.24</v>
+        <v>1</v>
       </c>
       <c r="E11" s="12">
-        <v>0.24</v>
+        <v>1</v>
       </c>
       <c r="F11" s="12">
-        <v>0.24</v>
+        <v>1</v>
       </c>
       <c r="G11" s="12">
-        <v>0.24</v>
+        <v>1</v>
       </c>
       <c r="H11" s="12">
-        <v>0.24</v>
+        <v>1</v>
       </c>
       <c r="I11" s="12">
-        <v>0.24</v>
+        <v>1</v>
       </c>
       <c r="J11" s="12">
-        <v>0.24</v>
+        <v>1</v>
       </c>
       <c r="K11" s="12">
-        <v>0.24</v>
+        <v>1</v>
       </c>
       <c r="L11" s="12">
-        <v>0.24</v>
+        <v>1</v>
       </c>
       <c r="M11" s="13">
-        <v>0.24</v>
+        <v>1</v>
       </c>
       <c r="N11" s="6"/>
       <c r="O11" s="10">
-        <v>0.24</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -3698,23 +3698,23 @@
         <v>103957033.9920633</v>
       </c>
       <c r="I12" s="17">
-        <v>234246685.647068</v>
+        <v>223552803.8082808</v>
       </c>
       <c r="J12" s="17">
-        <v>312711753.5362908</v>
+        <v>0</v>
       </c>
       <c r="K12" s="17">
-        <v>356766585.3744836</v>
+        <v>0</v>
       </c>
       <c r="L12" s="17">
-        <v>392308861.8314409</v>
+        <v>0</v>
       </c>
       <c r="M12" s="18">
-        <v>415206622.400336</v>
+        <v>0</v>
       </c>
       <c r="N12" s="6"/>
       <c r="O12" s="15">
-        <v>422310807.7096057</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -3784,23 +3784,23 @@
         <v>75753674.85386515</v>
       </c>
       <c r="I14" s="21">
-        <v>80867192.17195399</v>
+        <v>80960104.13287847</v>
       </c>
       <c r="J14" s="21">
-        <v>80661380.26485984</v>
+        <v>80905686.38168681</v>
       </c>
       <c r="K14" s="21">
-        <v>73753951.9928793</v>
+        <v>74204831.81714268</v>
       </c>
       <c r="L14" s="21">
-        <v>59502743.3347619</v>
+        <v>60195269.95737882</v>
       </c>
       <c r="M14" s="22">
-        <v>38334054.70585981</v>
+        <v>39265241.52367447</v>
       </c>
       <c r="N14" s="6"/>
       <c r="O14" s="19">
-        <v>11893400.11948828</v>
+        <v>13008855.92317652</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -3827,23 +3827,23 @@
         <v>28203359.1381982</v>
       </c>
       <c r="I15" s="17">
-        <v>153379493.475114</v>
+        <v>142592699.6754023</v>
       </c>
       <c r="J15" s="17">
-        <v>232050373.271431</v>
+        <v>-80905686.38168681</v>
       </c>
       <c r="K15" s="17">
-        <v>283012633.3816043</v>
+        <v>-74204831.81714268</v>
       </c>
       <c r="L15" s="17">
-        <v>332806118.496679</v>
+        <v>-60195269.95737882</v>
       </c>
       <c r="M15" s="18">
-        <v>376872567.6944762</v>
+        <v>-39265241.52367447</v>
       </c>
       <c r="N15" s="6"/>
       <c r="O15" s="15">
-        <v>410417407.5901174</v>
+        <v>-13008855.92317652</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -3855,38 +3855,38 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="11">
-        <v>0.06628929678467285</v>
+        <v>0.07258127135787265</v>
       </c>
       <c r="E16" s="12">
-        <v>0.06628929678467285</v>
+        <v>0.07258127135787265</v>
       </c>
       <c r="F16" s="12">
-        <v>0.06628929678467285</v>
+        <v>0.07258127135787265</v>
       </c>
       <c r="G16" s="12">
-        <v>0.06628929678467285</v>
+        <v>0.07258127135787265</v>
       </c>
       <c r="H16" s="12">
-        <v>0.06628929678467285</v>
+        <v>0.07258127135787265</v>
       </c>
       <c r="I16" s="12">
-        <v>0.06594102205261679</v>
+        <v>0.07183699874471659</v>
       </c>
       <c r="J16" s="12">
-        <v>0.06559274732056071</v>
+        <v>0.07109272613156055</v>
       </c>
       <c r="K16" s="12">
-        <v>0.06524447258850463</v>
+        <v>0.07034845351840449</v>
       </c>
       <c r="L16" s="12">
-        <v>0.06489619785644857</v>
+        <v>0.06960418090524843</v>
       </c>
       <c r="M16" s="13">
-        <v>0.0645479231243925</v>
+        <v>0.06885990829209239</v>
       </c>
       <c r="N16" s="6"/>
       <c r="O16" s="10">
-        <v>0.06419964839233643</v>
+        <v>0.06811563567893633</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -3898,34 +3898,34 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="11">
-        <v>0.9378317901299732</v>
+        <v>0.9323302827523869</v>
       </c>
       <c r="E17" s="12">
-        <v>0.87952846657839</v>
+        <v>0.8692397561371458</v>
       </c>
       <c r="F17" s="12">
-        <v>0.8248497562814818</v>
+        <v>0.8104185476189609</v>
       </c>
       <c r="G17" s="12">
-        <v>0.7735703235217342</v>
+        <v>0.7555777536493645</v>
       </c>
       <c r="H17" s="12">
-        <v>0.7254788412998104</v>
+        <v>0.7044480207013254</v>
       </c>
       <c r="I17" s="12">
-        <v>0.6805994199405148</v>
+        <v>0.657234282382807</v>
       </c>
       <c r="J17" s="12">
-        <v>0.6387050040007179</v>
+        <v>0.6136110033689838</v>
       </c>
       <c r="K17" s="12">
-        <v>0.5995853725940379</v>
+        <v>0.573281534020017</v>
       </c>
       <c r="L17" s="12">
-        <v>0.5630458384591434</v>
+        <v>0.5359754049716093</v>
       </c>
       <c r="M17" s="13">
-        <v>0.528906051318604</v>
+        <v>0.5014458871677885</v>
       </c>
       <c r="N17" s="6"/>
       <c r="O17" s="10" t="s">
@@ -3941,38 +3941,38 @@
       </c>
       <c r="C18" s="6"/>
       <c r="D18" s="16">
-        <v>-122056096.4368885</v>
+        <v>-121340091.1552443</v>
       </c>
       <c r="E18" s="17">
-        <v>-105505496.7557625</v>
+        <v>-104271295.0814237</v>
       </c>
       <c r="F18" s="17">
-        <v>-78573146.59173</v>
+        <v>-77198465.36632977</v>
       </c>
       <c r="G18" s="17">
-        <v>-37969196.12066755</v>
+        <v>-37086065.79181954</v>
       </c>
       <c r="H18" s="17">
-        <v>20460940.30834245</v>
+        <v>19867800.52203236</v>
       </c>
       <c r="I18" s="17">
-        <v>104389994.2899325</v>
+        <v>93716810.64419013</v>
       </c>
       <c r="J18" s="17">
-        <v>148211734.5886974</v>
+        <v>-49644619.39892317</v>
       </c>
       <c r="K18" s="17">
-        <v>169690235.2349291</v>
+        <v>-42540259.81582893</v>
       </c>
       <c r="L18" s="17">
-        <v>187385100.0332957</v>
+        <v>-32263184.19278146</v>
       </c>
       <c r="M18" s="18">
-        <v>199330181.6295887</v>
+        <v>-19689393.87069643</v>
       </c>
       <c r="N18" s="6"/>
       <c r="O18" s="15">
-        <v>4609765794.646161</v>
+        <v>-131874122.5074955</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -3986,7 +3986,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="19">
-        <v>485364250.1797373</v>
+        <v>-370448763.5068248</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -3994,7 +3994,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="19">
-        <v>4609765794.646161</v>
+        <v>-131874122.5074955</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -4002,7 +4002,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="15">
-        <v>5095130044.825898</v>
+        <v>-502322886.0143203</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -4042,7 +4042,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="15">
-        <v>5361367036.825898</v>
+        <v>-236085894.0143203</v>
       </c>
     </row>
     <row r="29" spans="1:15">
@@ -4050,7 +4050,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="19">
-        <v>3878781440</v>
+        <v>3618460416</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -4066,7 +4066,7 @@
         <v>29</v>
       </c>
       <c r="B31" s="26">
-        <v>56.95723310129354</v>
+        <v>-2.508091538023455</v>
       </c>
     </row>
     <row r="32" spans="1:15">
@@ -4074,7 +4074,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="28">
-        <v>34.27</v>
+        <v>31.97</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -4082,7 +4082,7 @@
         <v>31</v>
       </c>
       <c r="B33" s="30">
-        <v>1.66201438871589</v>
+        <v>-0.07845140875894449</v>
       </c>
     </row>
   </sheetData>

</xml_diff>